<commit_message>
Added tests of other apps
</commit_message>
<xml_diff>
--- a/experiments/lambda/analysis_run_cold.xlsx
+++ b/experiments/lambda/analysis_run_cold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimedantas/Documents/git/serverless-iot-deployment/experiments/lambda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B934BD-5228-664A-A0E7-0E2996703434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC7BB7-6AAD-9145-8C6A-9EF2853ABBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5860" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
+    <workbookView xWindow="-5860" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
   </bookViews>
   <sheets>
     <sheet name="run time" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,24 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'cold start bk'!$A$40</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'cold start bk'!$A$41:$A$52</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'cold start bk'!$B$40</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'cold start bk'!$B$41:$B$52</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">resize!$A$3:$A$9</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">resize!$AE$3:$AE$9</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">resize!$K$3:$K$9</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">resize!$P$3:$P$9</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">resize!$U$3:$U$9</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">resize!$Z$3:$Z$9</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'cold start bk'!$A$40</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'cold start bk'!$A$41:$A$52</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'cold start bk'!$B$40</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'cold start bk'!$B$41:$B$52</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">resize!$F$3:$F$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">resize!$K$3:$K$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">resize!$P$3:$P$9</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">resize!$U$3:$U$9</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">resize!$Z$3:$Z$9</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">resize!$A$3:$A$9</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">resize!$AE$3:$AE$9</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">resize!$F$3:$F$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
   <si>
     <t>Memory</t>
   </si>
@@ -102,6 +116,18 @@
   <si>
     <t>Zip 241MB</t>
   </si>
+  <si>
+    <t>math scipy zip</t>
+  </si>
+  <si>
+    <t>opencv zip</t>
+  </si>
+  <si>
+    <t>tensorflow zip</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +158,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +192,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -294,6 +338,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,6 +398,37 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4522,7 +4606,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cold Start - AVerage</a:t>
+              <a:t>Cold Start Improvement of the image container - AVerage</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4559,28 +4643,26 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Resize - Zip</c:v>
+            <c:v>Resize</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>resize!$A$3:$A$9</c:f>
@@ -4613,35 +4695,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>resize!$B$3:$B$9</c:f>
+              <c:f>resize!$F$3:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>353.15</c:v>
+                  <c:v>5.5833934022036735E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>229.95</c:v>
+                  <c:v>2.6579607416876594E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>166.55</c:v>
+                  <c:v>-7.9280134913822131E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>129.05000000000001</c:v>
+                  <c:v>-3.8883380787015254E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.3</c:v>
+                  <c:v>-0.13318749591514267</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.7</c:v>
+                  <c:v>-0.14232110718782964</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.650000000000006</c:v>
+                  <c:v>-0.1277446801298292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E1E6-234E-98F5-17CBF2924811}"/>
@@ -4649,140 +4730,51 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Resize - Image</c:v>
+            <c:v>Resize + Feature</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:invertIfNegative val="0"/>
+          <c:val>
             <c:numRef>
-              <c:f>resize!$A$3:$A$9</c:f>
+              <c:f>resize!$K$3:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>6.2411719344502403E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>192</c:v>
+                  <c:v>6.1931890775252851E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256</c:v>
+                  <c:v>6.8002842663328344E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>320</c:v>
+                  <c:v>1.7048549794708157E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>384</c:v>
+                  <c:v>4.2218045435103102E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>448</c:v>
+                  <c:v>3.0868132930943148E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>resize!$D$3:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>485.95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>381.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>354.55</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>302.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>294.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>291.64999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>266.14999999999998</c:v>
+                  <c:v>4.3051411386417437E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E1E6-234E-98F5-17CBF2924811}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Resize + Feature - Zip</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>resize!$F$3:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>378.15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>243.45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>182.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>141.19999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>117.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>97.65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>81.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-E1E6-234E-98F5-17CBF2924811}"/>
@@ -4790,58 +4782,210 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Resize + Feature - Image</c:v>
+            <c:v>TensorFlow</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>resize!$H$3:$H$9</c:f>
+              <c:f>resize!$Z$3:$Z$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>736.8</c:v>
+                  <c:v>0.14793472775325645</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>609.4</c:v>
+                  <c:v>0.13277589431743808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>550.15</c:v>
+                  <c:v>0.14634669477451423</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>537.70000000000005</c:v>
+                  <c:v>0.14880437199408048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>502.7</c:v>
+                  <c:v>0.15546448573519356</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>491</c:v>
+                  <c:v>0.15739746637150331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>466.8</c:v>
+                  <c:v>0.13742937220313645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-712B-2A42-B0AA-800A7DD2E896}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>OpenCV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>resize!$U$3:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.38039275930050953</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35172752844815802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3234057044223313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30116463299856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2768007822509152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2520008800907555</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24972109110278617</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-712B-2A42-B0AA-800A7DD2E896}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Math Scipy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>resize!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.21016725493084965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19360501055261359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18418994717230208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18707655305307913</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17635508311291204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17465441862189512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18331991640071821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-E1E6-234E-98F5-17CBF2924811}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Image Classifier</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>resize!$AE$3:$AE$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.78039663615213872</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7518960616675181</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69905994539159844</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67255007100918296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63786651340742584</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59390548247701713</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55889683489699782</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-712B-2A42-B0AA-800A7DD2E896}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4853,10 +4997,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="192646799"/>
         <c:axId val="192633263"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="192646799"/>
         <c:scaling>
@@ -4981,8 +5125,8 @@
         <c:axId val="192633263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="800"/>
-          <c:min val="0"/>
+          <c:max val="1"/>
+          <c:min val="-0.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5007,7 +5151,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>time (ms)</a:t>
+                  <a:t>savings (time)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5041,7 +5185,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5081,6 +5225,7 @@
         <c:crossAx val="192646799"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -6592,12 +6737,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6635,7 +6780,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1027A42A-5AA0-674F-AD44-EB53C8071287}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>Zip Package	</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6656,7 +6801,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A791611B-19A8-E44E-966E-83FC41317DC0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>Image Container	</cx:v>
             </cx:txData>
           </cx:tx>
@@ -12616,16 +12761,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1044348</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>112258</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>272051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>155162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>48759</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>614405</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>91663</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13124,24 +13269,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -13506,10 +13651,10 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13519,52 +13664,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="37" t="s">
+      <c r="I1" s="44"/>
+      <c r="J1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="37"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="40"/>
+      <c r="L1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="43" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="43"/>
-      <c r="P1" s="44" t="s">
+      <c r="O1" s="46"/>
+      <c r="P1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="45" t="s">
+      <c r="Q1" s="47"/>
+      <c r="R1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="45"/>
-      <c r="T1" s="46" t="s">
+      <c r="S1" s="48"/>
+      <c r="T1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="46"/>
+      <c r="U1" s="49"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14198,10 +14343,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DE693F-DFBF-A645-98AD-B3E2E7E6F16B}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14210,29 +14356,67 @@
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="44"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="51"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="52"/>
+      <c r="S1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="53"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="54"/>
+      <c r="X1" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="41"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14245,28 +14429,94 @@
       <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="K2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>128</v>
       </c>
       <c r="B3" s="21">
-        <v>353.15</v>
+        <v>514.68700000000001</v>
       </c>
       <c r="C3" s="21">
-        <v>369.05</v>
+        <v>534.60900000000004</v>
       </c>
       <c r="D3" s="21">
         <v>485.95</v>
@@ -14274,28 +14524,100 @@
       <c r="E3" s="21">
         <v>519.1</v>
       </c>
-      <c r="F3" s="25">
-        <v>378.15</v>
+      <c r="F3" s="27">
+        <f>1-D3/B3</f>
+        <v>5.5833934022036735E-2</v>
       </c>
       <c r="G3" s="25">
-        <v>403</v>
-      </c>
-      <c r="H3" s="21">
+        <v>785.84599999999978</v>
+      </c>
+      <c r="H3" s="25">
+        <v>821.59649999999999</v>
+      </c>
+      <c r="I3" s="21">
         <v>736.8</v>
       </c>
-      <c r="I3" s="21">
+      <c r="J3" s="21">
         <v>771.30000000000007</v>
       </c>
+      <c r="K3" s="27">
+        <f>1-I3/G3</f>
+        <v>6.2411719344502403E-2</v>
+      </c>
+      <c r="L3">
+        <v>1170.8175000000001</v>
+      </c>
+      <c r="M3">
+        <v>1206.662</v>
+      </c>
+      <c r="N3">
+        <v>924.75</v>
+      </c>
+      <c r="O3">
+        <v>1145.5500000000002</v>
+      </c>
+      <c r="P3" s="27">
+        <f>1-N3/L3</f>
+        <v>0.21016725493084965</v>
+      </c>
+      <c r="Q3">
+        <v>1054.539</v>
+      </c>
+      <c r="R3">
+        <v>1084.4325000000001</v>
+      </c>
+      <c r="S3">
+        <v>653.4</v>
+      </c>
+      <c r="T3">
+        <v>696.05000000000007</v>
+      </c>
+      <c r="U3" s="27">
+        <f>1-S3/Q3</f>
+        <v>0.38039275930050953</v>
+      </c>
+      <c r="V3">
+        <v>6716.2694999999994</v>
+      </c>
+      <c r="W3">
+        <v>6907.2835000000005</v>
+      </c>
+      <c r="X3">
+        <v>5722.7</v>
+      </c>
+      <c r="Y3">
+        <v>5841.7</v>
+      </c>
+      <c r="Z3" s="27">
+        <f>1-X3/V3</f>
+        <v>0.14793472775325645</v>
+      </c>
+      <c r="AA3" s="21">
+        <v>12584.279</v>
+      </c>
+      <c r="AB3" s="21">
+        <v>12847.5445</v>
+      </c>
+      <c r="AC3" s="21">
+        <v>2763.55</v>
+      </c>
+      <c r="AD3" s="21">
+        <v>3719.4500000000003</v>
+      </c>
+      <c r="AE3" s="27">
+        <f>1-AC3/AA3</f>
+        <v>0.78039663615213872</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>192</v>
       </c>
       <c r="B4" s="21">
-        <v>229.95</v>
+        <v>391.91700000000003</v>
       </c>
       <c r="C4" s="21">
-        <v>240.2</v>
+        <v>410.25600000000003</v>
       </c>
       <c r="D4" s="21">
         <v>381.5</v>
@@ -14303,28 +14625,100 @@
       <c r="E4" s="21">
         <v>398.1</v>
       </c>
-      <c r="F4" s="21">
-        <v>243.45</v>
+      <c r="F4" s="27">
+        <f t="shared" ref="F4:F9" si="0">1-D4/B4</f>
+        <v>2.6579607416876594E-2</v>
       </c>
       <c r="G4" s="21">
-        <v>255</v>
+        <v>649.63299999999981</v>
       </c>
       <c r="H4" s="21">
+        <v>674.25350000000003</v>
+      </c>
+      <c r="I4" s="21">
         <v>609.4</v>
       </c>
-      <c r="I4" s="21">
+      <c r="J4" s="21">
         <v>649.15</v>
       </c>
+      <c r="K4" s="27">
+        <f t="shared" ref="K4:K9" si="1">1-I4/G4</f>
+        <v>6.1931890775252851E-2</v>
+      </c>
+      <c r="L4">
+        <v>1089.5404999999998</v>
+      </c>
+      <c r="M4">
+        <v>1106.6965</v>
+      </c>
+      <c r="N4">
+        <v>878.6</v>
+      </c>
+      <c r="O4">
+        <v>913.00000000000011</v>
+      </c>
+      <c r="P4" s="27">
+        <f t="shared" ref="P4:P9" si="2">1-N4/L4</f>
+        <v>0.19360501055261359</v>
+      </c>
+      <c r="Q4">
+        <v>862.44600000000014</v>
+      </c>
+      <c r="R4">
+        <v>906.14</v>
+      </c>
+      <c r="S4">
+        <v>559.1</v>
+      </c>
+      <c r="T4">
+        <v>587.75</v>
+      </c>
+      <c r="U4" s="27">
+        <f t="shared" ref="U4:U9" si="3">1-S4/Q4</f>
+        <v>0.35172752844815802</v>
+      </c>
+      <c r="V4">
+        <v>4632.1360000000004</v>
+      </c>
+      <c r="W4">
+        <v>4697.8755000000001</v>
+      </c>
+      <c r="X4">
+        <v>4017.1</v>
+      </c>
+      <c r="Y4">
+        <v>4203.9500000000007</v>
+      </c>
+      <c r="Z4" s="27">
+        <f t="shared" ref="Z4:Z9" si="4">1-X4/V4</f>
+        <v>0.13277589431743808</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>8680.031500000001</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>9072.0564999999988</v>
+      </c>
+      <c r="AC4" s="21">
+        <v>2153.5500000000002</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>2320.15</v>
+      </c>
+      <c r="AE4" s="27">
+        <f t="shared" ref="AE4:AE9" si="5">1-AC4/AA4</f>
+        <v>0.7518960616675181</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>256</v>
       </c>
       <c r="B5" s="21">
-        <v>166.55</v>
+        <v>328.50599999999997</v>
       </c>
       <c r="C5" s="21">
-        <v>180.05</v>
+        <v>347.40950000000004</v>
       </c>
       <c r="D5" s="21">
         <v>354.55</v>
@@ -14332,28 +14726,100 @@
       <c r="E5" s="21">
         <v>376.90000000000015</v>
       </c>
-      <c r="F5" s="21">
-        <v>182.6</v>
+      <c r="F5" s="27">
+        <f t="shared" si="0"/>
+        <v>-7.9280134913822131E-2</v>
       </c>
       <c r="G5" s="21">
-        <v>201.5</v>
+        <v>590.29150000000004</v>
       </c>
       <c r="H5" s="21">
+        <v>620.77499999999998</v>
+      </c>
+      <c r="I5" s="21">
         <v>550.15</v>
       </c>
-      <c r="I5" s="21">
+      <c r="J5" s="21">
         <v>588.15000000000009</v>
       </c>
+      <c r="K5" s="27">
+        <f t="shared" si="1"/>
+        <v>6.8002842663328344E-2</v>
+      </c>
+      <c r="L5">
+        <v>1066.4859999999996</v>
+      </c>
+      <c r="M5">
+        <v>1093.9804999999999</v>
+      </c>
+      <c r="N5">
+        <v>870.05</v>
+      </c>
+      <c r="O5">
+        <v>901.05000000000007</v>
+      </c>
+      <c r="P5" s="27">
+        <f t="shared" si="2"/>
+        <v>0.18418994717230208</v>
+      </c>
+      <c r="Q5">
+        <v>769.36800000000017</v>
+      </c>
+      <c r="R5">
+        <v>795.572</v>
+      </c>
+      <c r="S5">
+        <v>520.54999999999995</v>
+      </c>
+      <c r="T5">
+        <v>549</v>
+      </c>
+      <c r="U5" s="27">
+        <f t="shared" si="3"/>
+        <v>0.3234057044223313</v>
+      </c>
+      <c r="V5">
+        <v>3589.982</v>
+      </c>
+      <c r="W5">
+        <v>3652.1385</v>
+      </c>
+      <c r="X5">
+        <v>3064.6</v>
+      </c>
+      <c r="Y5">
+        <v>3125</v>
+      </c>
+      <c r="Z5" s="27">
+        <f t="shared" si="4"/>
+        <v>0.14634669477451423</v>
+      </c>
+      <c r="AA5" s="21">
+        <v>6297.9319999999998</v>
+      </c>
+      <c r="AB5" s="21">
+        <v>6455.8615</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>1895.3</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>2060.4500000000003</v>
+      </c>
+      <c r="AE5" s="27">
+        <f t="shared" si="5"/>
+        <v>0.69905994539159844</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>320</v>
       </c>
       <c r="B6" s="21">
-        <v>129.05000000000001</v>
+        <v>290.9855</v>
       </c>
       <c r="C6" s="21">
-        <v>141</v>
+        <v>305.50300000000004</v>
       </c>
       <c r="D6" s="21">
         <v>302.3</v>
@@ -14361,28 +14827,100 @@
       <c r="E6" s="21">
         <v>310.35000000000002</v>
       </c>
-      <c r="F6" s="21">
-        <v>141.19999999999999</v>
+      <c r="F6" s="27">
+        <f t="shared" si="0"/>
+        <v>-3.8883380787015254E-2</v>
       </c>
       <c r="G6" s="21">
-        <v>158.05000000000001</v>
+        <v>547.02600000000007</v>
       </c>
       <c r="H6" s="21">
+        <v>577.76049999999998</v>
+      </c>
+      <c r="I6" s="21">
         <v>537.70000000000005</v>
       </c>
-      <c r="I6" s="21">
+      <c r="J6" s="21">
         <v>692.80000000000007</v>
       </c>
+      <c r="K6" s="27">
+        <f t="shared" si="1"/>
+        <v>1.7048549794708157E-2</v>
+      </c>
+      <c r="L6">
+        <v>1056.0650000000001</v>
+      </c>
+      <c r="M6">
+        <v>1085.9730000000002</v>
+      </c>
+      <c r="N6">
+        <v>858.5</v>
+      </c>
+      <c r="O6">
+        <v>881.3</v>
+      </c>
+      <c r="P6" s="27">
+        <f t="shared" si="2"/>
+        <v>0.18707655305307913</v>
+      </c>
+      <c r="Q6">
+        <v>719.84049999999991</v>
+      </c>
+      <c r="R6">
+        <v>746.03300000000002</v>
+      </c>
+      <c r="S6">
+        <v>503.05</v>
+      </c>
+      <c r="T6">
+        <v>521.29999999999995</v>
+      </c>
+      <c r="U6" s="27">
+        <f t="shared" si="3"/>
+        <v>0.30116463299856</v>
+      </c>
+      <c r="V6">
+        <v>2952.6115</v>
+      </c>
+      <c r="W6">
+        <v>3029.2019999999998</v>
+      </c>
+      <c r="X6">
+        <v>2513.25</v>
+      </c>
+      <c r="Y6">
+        <v>2613.4</v>
+      </c>
+      <c r="Z6" s="27">
+        <f t="shared" si="4"/>
+        <v>0.14880437199408048</v>
+      </c>
+      <c r="AA6" s="21">
+        <v>5348.6040000000003</v>
+      </c>
+      <c r="AB6" s="21">
+        <v>5556.4615000000003</v>
+      </c>
+      <c r="AC6" s="21">
+        <v>1751.4</v>
+      </c>
+      <c r="AD6" s="21">
+        <v>2203</v>
+      </c>
+      <c r="AE6" s="27">
+        <f t="shared" si="5"/>
+        <v>0.67255007100918296</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>384</v>
       </c>
       <c r="B7" s="21">
-        <v>97.3</v>
+        <v>260.10699999999997</v>
       </c>
       <c r="C7" s="21">
-        <v>119</v>
+        <v>283.09449999999998</v>
       </c>
       <c r="D7" s="21">
         <v>294.75</v>
@@ -14390,28 +14928,100 @@
       <c r="E7" s="21">
         <v>314.25000000000006</v>
       </c>
-      <c r="F7" s="21">
-        <v>117.5</v>
+      <c r="F7" s="27">
+        <f t="shared" si="0"/>
+        <v>-0.13318749591514267</v>
       </c>
       <c r="G7" s="21">
-        <v>125</v>
+        <v>524.85850000000005</v>
       </c>
       <c r="H7" s="21">
+        <v>548.50099999999998</v>
+      </c>
+      <c r="I7" s="21">
         <v>502.7</v>
       </c>
-      <c r="I7" s="21">
+      <c r="J7" s="21">
         <v>668.45</v>
       </c>
+      <c r="K7" s="27">
+        <f t="shared" si="1"/>
+        <v>4.2218045435103102E-2</v>
+      </c>
+      <c r="L7">
+        <v>1045.5355</v>
+      </c>
+      <c r="M7">
+        <v>1075.5204999999999</v>
+      </c>
+      <c r="N7">
+        <v>861.15</v>
+      </c>
+      <c r="O7">
+        <v>903.80000000000007</v>
+      </c>
+      <c r="P7" s="27">
+        <f t="shared" si="2"/>
+        <v>0.17635508311291204</v>
+      </c>
+      <c r="Q7">
+        <v>679.06600000000003</v>
+      </c>
+      <c r="R7">
+        <v>697.84749999999997</v>
+      </c>
+      <c r="S7">
+        <v>491.1</v>
+      </c>
+      <c r="T7">
+        <v>512.25</v>
+      </c>
+      <c r="U7" s="27">
+        <f t="shared" si="3"/>
+        <v>0.2768007822509152</v>
+      </c>
+      <c r="V7">
+        <v>2557.5005000000006</v>
+      </c>
+      <c r="W7">
+        <v>2635.422</v>
+      </c>
+      <c r="X7">
+        <v>2159.9</v>
+      </c>
+      <c r="Y7">
+        <v>2260.6</v>
+      </c>
+      <c r="Z7" s="27">
+        <f t="shared" si="4"/>
+        <v>0.15546448573519356</v>
+      </c>
+      <c r="AA7" s="21">
+        <v>4442.1464999999998</v>
+      </c>
+      <c r="AB7" s="21">
+        <v>4542.6000000000004</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>1608.65</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>1722.25</v>
+      </c>
+      <c r="AE7" s="27">
+        <f t="shared" si="5"/>
+        <v>0.63786651340742584</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>448</v>
       </c>
       <c r="B8" s="21">
-        <v>92.7</v>
+        <v>255.31350000000003</v>
       </c>
       <c r="C8" s="21">
-        <v>102.05</v>
+        <v>263.99249999999995</v>
       </c>
       <c r="D8" s="21">
         <v>291.64999999999998</v>
@@ -14419,28 +15029,100 @@
       <c r="E8" s="21">
         <v>310.30000000000013</v>
       </c>
-      <c r="F8" s="21">
-        <v>97.65</v>
+      <c r="F8" s="27">
+        <f t="shared" si="0"/>
+        <v>-0.14232110718782964</v>
       </c>
       <c r="G8" s="21">
-        <v>105.05</v>
+        <v>506.63900000000012</v>
       </c>
       <c r="H8" s="21">
+        <v>528.33649999999989</v>
+      </c>
+      <c r="I8" s="21">
         <v>491</v>
       </c>
-      <c r="I8" s="21">
+      <c r="J8" s="21">
         <v>657.8</v>
       </c>
+      <c r="K8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.0868132930943148E-2</v>
+      </c>
+      <c r="L8">
+        <v>1051.9229999999998</v>
+      </c>
+      <c r="M8">
+        <v>1082.8644999999999</v>
+      </c>
+      <c r="N8">
+        <v>868.2</v>
+      </c>
+      <c r="O8">
+        <v>908.10000000000014</v>
+      </c>
+      <c r="P8" s="27">
+        <f t="shared" si="2"/>
+        <v>0.17465441862189512</v>
+      </c>
+      <c r="Q8">
+        <v>640.84300000000007</v>
+      </c>
+      <c r="R8">
+        <v>661.35750000000007</v>
+      </c>
+      <c r="S8">
+        <v>479.35</v>
+      </c>
+      <c r="T8">
+        <v>501.1</v>
+      </c>
+      <c r="U8" s="27">
+        <f t="shared" si="3"/>
+        <v>0.2520008800907555</v>
+      </c>
+      <c r="V8">
+        <v>2241.9229999999998</v>
+      </c>
+      <c r="W8">
+        <v>2280.6129999999998</v>
+      </c>
+      <c r="X8">
+        <v>1889.05</v>
+      </c>
+      <c r="Y8">
+        <v>2013.9</v>
+      </c>
+      <c r="Z8" s="27">
+        <f t="shared" si="4"/>
+        <v>0.15739746637150331</v>
+      </c>
+      <c r="AA8" s="21">
+        <v>3855.1370000000011</v>
+      </c>
+      <c r="AB8" s="21">
+        <v>3950.585</v>
+      </c>
+      <c r="AC8" s="21">
+        <v>1565.55</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>1715.3</v>
+      </c>
+      <c r="AE8" s="27">
+        <f t="shared" si="5"/>
+        <v>0.59390548247701713</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>512</v>
       </c>
       <c r="B9" s="21">
-        <v>73.650000000000006</v>
+        <v>236.00200000000004</v>
       </c>
       <c r="C9" s="21">
-        <v>82.1</v>
+        <v>247.209</v>
       </c>
       <c r="D9" s="21">
         <v>266.14999999999998</v>
@@ -14448,90 +15130,215 @@
       <c r="E9" s="21">
         <v>277.3</v>
       </c>
-      <c r="F9" s="21">
-        <v>81.8</v>
+      <c r="F9" s="27">
+        <f t="shared" si="0"/>
+        <v>-0.1277446801298292</v>
       </c>
       <c r="G9" s="21">
-        <v>99</v>
+        <v>487.80050000000011</v>
       </c>
       <c r="H9" s="21">
+        <v>510.13650000000001</v>
+      </c>
+      <c r="I9" s="21">
         <v>466.8</v>
       </c>
-      <c r="I9" s="21">
+      <c r="J9" s="21">
         <v>571.85</v>
       </c>
+      <c r="K9" s="27">
+        <f t="shared" si="1"/>
+        <v>4.3051411386417437E-2</v>
+      </c>
+      <c r="L9">
+        <v>1045.942</v>
+      </c>
+      <c r="M9">
+        <v>1078.2284999999999</v>
+      </c>
+      <c r="N9">
+        <v>854.2</v>
+      </c>
+      <c r="O9">
+        <v>883.9</v>
+      </c>
+      <c r="P9" s="27">
+        <f t="shared" si="2"/>
+        <v>0.18331991640071821</v>
+      </c>
+      <c r="Q9">
+        <v>626.10050000000001</v>
+      </c>
+      <c r="R9">
+        <v>641.43700000000001</v>
+      </c>
+      <c r="S9">
+        <v>469.75</v>
+      </c>
+      <c r="T9">
+        <v>489.15</v>
+      </c>
+      <c r="U9" s="27">
+        <f t="shared" si="3"/>
+        <v>0.24972109110278617</v>
+      </c>
+      <c r="V9">
+        <v>2020.0084999999995</v>
+      </c>
+      <c r="W9">
+        <v>2065.1440000000002</v>
+      </c>
+      <c r="X9">
+        <v>1742.4</v>
+      </c>
+      <c r="Y9">
+        <v>1848.95</v>
+      </c>
+      <c r="Z9" s="27">
+        <f t="shared" si="4"/>
+        <v>0.13742937220313645</v>
+      </c>
+      <c r="AA9" s="21">
+        <v>3401.3584999999998</v>
+      </c>
+      <c r="AB9" s="21">
+        <v>3566.55</v>
+      </c>
+      <c r="AC9" s="21">
+        <v>1500.35</v>
+      </c>
+      <c r="AD9" s="21">
+        <v>1640.2</v>
+      </c>
+      <c r="AE9" s="27">
+        <f t="shared" si="5"/>
+        <v>0.55889683489699782</v>
+      </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q34" s="2"/>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="56"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="Q35" s="2"/>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="27"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="Q36" s="2"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="27"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="27"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="27"/>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="27"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="Q37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="Q38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="Q39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="Q40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="Q41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="Q42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="Q43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="Q44" s="22"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="Q45" s="23"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" s="22"/>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
       <c r="B46" s="2"/>
+      <c r="T46" s="23"/>
+      <c r="U46" s="23"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="22"/>
       <c r="B47" s="2"/>
     </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A48" s="23"/>
+      <c r="B48" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14553,20 +15360,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added new tests and analysis for paper 1
</commit_message>
<xml_diff>
--- a/experiments/lambda/analysis_run_cold.xlsx
+++ b/experiments/lambda/analysis_run_cold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimedantas/Documents/git/serverless-iot-deployment/experiments/lambda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC7BB7-6AAD-9145-8C6A-9EF2853ABBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7E83C9-2BC6-1645-A3D6-AC379247C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5860" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
   </bookViews>
   <sheets>
     <sheet name="run time" sheetId="2" r:id="rId1"/>
@@ -20,24 +20,10 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">resize!$A$3:$A$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">resize!$AE$3:$AE$9</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">resize!$K$3:$K$9</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">resize!$P$3:$P$9</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">resize!$U$3:$U$9</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">resize!$Z$3:$Z$9</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'cold start bk'!$A$40</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'cold start bk'!$A$41:$A$52</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'cold start bk'!$B$40</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'cold start bk'!$B$41:$B$52</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">resize!$F$3:$F$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">resize!$K$3:$K$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">resize!$P$3:$P$9</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">resize!$U$3:$U$9</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">resize!$Z$3:$Z$9</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">resize!$A$3:$A$9</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">resize!$AE$3:$AE$9</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">resize!$F$3:$F$9</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'cold start bk'!$A$40</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'cold start bk'!$A$41:$A$52</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'cold start bk'!$B$40</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'cold start bk'!$B$41:$B$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="24">
   <si>
     <t>Memory</t>
   </si>
@@ -128,6 +114,9 @@
   <si>
     <t>diff</t>
   </si>
+  <si>
+    <t>factorial zip</t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,8 +146,14 @@
       <name val="Monaco"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +205,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -348,6 +355,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -369,6 +392,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -383,25 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -416,19 +436,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2357,7 +2380,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$P$3:$P$9</c:f>
+              <c:f>'cold start'!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2461,7 +2484,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$T$3:$T$9</c:f>
+              <c:f>'cold start'!$U$3:$U$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2587,25 +2610,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.128450000000001</c:v>
+                  <c:v>12.584279</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2236000000000011</c:v>
+                  <c:v>8.6800315000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8582000000000001</c:v>
+                  <c:v>6.2979319999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8888999999999996</c:v>
+                  <c:v>5.3486039999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9879499999999997</c:v>
+                  <c:v>4.4421464999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.39845</c:v>
+                  <c:v>3.8551370000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9441999999999999</c:v>
+                  <c:v>3.4013584999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2637,30 +2660,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$N$3:$N$9</c:f>
+              <c:f>'cold start'!$O$3:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.69225</c:v>
+                  <c:v>13.131603500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5152000000000001</c:v>
+                  <c:v>8.9549250000000011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3908500000000004</c:v>
+                  <c:v>6.8351664999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0598000000000001</c:v>
+                  <c:v>5.5005895000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1367500000000001</c:v>
+                  <c:v>4.5758350000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5381</c:v>
+                  <c:v>3.9798525000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0644499999999999</c:v>
+                  <c:v>3.5054605000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2787,30 +2810,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$R$3:$R$9</c:f>
+              <c:f>'cold start'!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.0905</c:v>
+                  <c:v>14.531919</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5402999999999984</c:v>
+                  <c:v>9.9824789999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1855500000000001</c:v>
+                  <c:v>7.627080499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6292999999999997</c:v>
+                  <c:v>6.0706370000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5728999999999997</c:v>
+                  <c:v>5.0136354999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9009499999999999</c:v>
+                  <c:v>4.3454945</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3694499999999996</c:v>
+                  <c:v>3.8091395000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2847,25 +2870,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.8401</c:v>
+                  <c:v>15.284255999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.42825</c:v>
+                  <c:v>10.867018499999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3516000000000004</c:v>
+                  <c:v>7.7882359999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0501000000000005</c:v>
+                  <c:v>6.4936315000000011</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7641999999999998</c:v>
+                  <c:v>5.2042145000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.06175</c:v>
+                  <c:v>4.5009115000000008</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5368000000000004</c:v>
+                  <c:v>3.9799080000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3014,7 +3037,7 @@
         <c:axId val="192633263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15"/>
+          <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3476,7 +3499,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$P$3:$P$9</c:f>
+              <c:f>'cold start'!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3531,7 +3554,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$T$3:$T$9</c:f>
+              <c:f>'cold start'!$U$3:$U$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4068,25 +4091,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.128450000000001</c:v>
+                  <c:v>12.584279</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2236000000000011</c:v>
+                  <c:v>8.6800315000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8582000000000001</c:v>
+                  <c:v>6.2979319999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8888999999999996</c:v>
+                  <c:v>5.3486039999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9879499999999997</c:v>
+                  <c:v>4.4421464999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.39845</c:v>
+                  <c:v>3.8551370000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9441999999999999</c:v>
+                  <c:v>3.4013584999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4123,25 +4146,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.8401</c:v>
+                  <c:v>15.284255999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.42825</c:v>
+                  <c:v>10.867018499999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3516000000000004</c:v>
+                  <c:v>7.7882359999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0501000000000005</c:v>
+                  <c:v>6.4936315000000011</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7641999999999998</c:v>
+                  <c:v>5.2042145000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.06175</c:v>
+                  <c:v>4.5009115000000008</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5368000000000004</c:v>
+                  <c:v>3.9799080000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4173,30 +4196,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$N$3:$N$9</c:f>
+              <c:f>'cold start'!$O$3:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.69225</c:v>
+                  <c:v>13.131603500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5152000000000001</c:v>
+                  <c:v>8.9549250000000011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3908500000000004</c:v>
+                  <c:v>6.8351664999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0598000000000001</c:v>
+                  <c:v>5.5005895000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1367500000000001</c:v>
+                  <c:v>4.5758350000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5381</c:v>
+                  <c:v>3.9798525000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0644499999999999</c:v>
+                  <c:v>3.5054605000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4228,30 +4251,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'cold start'!$R$3:$R$9</c:f>
+              <c:f>'cold start'!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.0905</c:v>
+                  <c:v>14.531919</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5402999999999984</c:v>
+                  <c:v>9.9824789999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1855500000000001</c:v>
+                  <c:v>7.627080499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6292999999999997</c:v>
+                  <c:v>6.0706370000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5728999999999997</c:v>
+                  <c:v>5.0136354999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9009499999999999</c:v>
+                  <c:v>4.3454945</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3694499999999996</c:v>
+                  <c:v>3.8091395000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4648,8 +4671,62 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Factorial</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>resize!$AJ$3:$AJ$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-9.3174136328073365E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.12696409891401639</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.16670224937456557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.1784779109338468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.21739903141244921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2570320537249895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.27706569106523049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-906A-2947-BA37-C28178F39CFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Resize</c:v>
           </c:tx>
@@ -4697,7 +4774,7 @@
             <c:numRef>
               <c:f>resize!$F$3:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5.5833934022036735E-2</c:v>
@@ -4731,7 +4808,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Resize + Feature</c:v>
           </c:tx>
@@ -4749,7 +4826,7 @@
             <c:numRef>
               <c:f>resize!$K$3:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>6.2411719344502403E-2</c:v>
@@ -4783,7 +4860,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>TensorFlow</c:v>
           </c:tx>
@@ -4801,7 +4878,7 @@
             <c:numRef>
               <c:f>resize!$Z$3:$Z$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.14793472775325645</c:v>
@@ -4835,7 +4912,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>OpenCV</c:v>
           </c:tx>
@@ -4853,7 +4930,7 @@
             <c:numRef>
               <c:f>resize!$U$3:$U$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.38039275930050953</c:v>
@@ -4887,7 +4964,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:v>Math Scipy</c:v>
           </c:tx>
@@ -4905,7 +4982,7 @@
             <c:numRef>
               <c:f>resize!$P$3:$P$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.21016725493084965</c:v>
@@ -4939,7 +5016,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>Image Classifier</c:v>
           </c:tx>
@@ -4957,7 +5034,7 @@
             <c:numRef>
               <c:f>resize!$AE$3:$AE$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.78039663615213872</c:v>
@@ -6737,12 +6814,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6780,7 +6857,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1027A42A-5AA0-674F-AD44-EB53C8071287}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Zip Package	</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6801,7 +6878,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A791611B-19A8-E44E-966E-83FC41317DC0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Image Container	</cx:v>
             </cx:txData>
           </cx:tx>
@@ -12643,15 +12720,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>160337</xdr:rowOff>
+      <xdr:colOff>327813</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122141</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1910</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>139605</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12680,16 +12757,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>629920</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>95183</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>135327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>589280</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>124143</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>54543</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152789</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12724,7 +12801,7 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>195263</xdr:rowOff>
@@ -13256,8 +13333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AD9F75-3855-FE49-9A21-1A6C70A44219}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="37" zoomScaleNormal="37" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13269,24 +13346,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="33"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -13648,13 +13725,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22115D20-AEC8-E342-9EA8-01B34B7AB9E3}">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:M9"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13663,53 +13740,54 @@
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="40" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="45" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46" t="s">
+      <c r="M1" s="48"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="49"/>
+      <c r="Q1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="50"/>
+      <c r="S1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="51"/>
+      <c r="U1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="49"/>
+      <c r="V1" s="52"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="54"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -13746,32 +13824,35 @@
       <c r="M2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>128</v>
       </c>
@@ -13788,10 +13869,10 @@
         <v>2.9409999999999998</v>
       </c>
       <c r="F3" s="21">
-        <v>12.128450000000001</v>
+        <v>12.584279</v>
       </c>
       <c r="G3" s="21">
-        <v>12.38785</v>
+        <v>12.8475445</v>
       </c>
       <c r="H3" s="21">
         <v>2.7635500000000004</v>
@@ -13800,10 +13881,10 @@
         <v>3.7194500000000001</v>
       </c>
       <c r="J3" s="21">
-        <v>14.8401</v>
+        <v>15.284255999999997</v>
       </c>
       <c r="K3" s="21">
-        <v>15.20805</v>
+        <v>15.6767825</v>
       </c>
       <c r="L3" s="21">
         <v>3.05945</v>
@@ -13811,32 +13892,36 @@
       <c r="M3" s="21">
         <v>3.1539999999999999</v>
       </c>
-      <c r="N3">
-        <v>12.69225</v>
+      <c r="N3" s="27">
+        <f>1-L3/J3</f>
+        <v>0.79982996882543711</v>
       </c>
       <c r="O3">
-        <v>12.989799999999999</v>
+        <v>13.131603500000001</v>
       </c>
       <c r="P3">
+        <v>13.437488999999999</v>
+      </c>
+      <c r="Q3">
         <v>2.8224499999999999</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2.992</v>
       </c>
-      <c r="R3">
-        <v>14.0905</v>
-      </c>
       <c r="S3">
-        <v>14.515549999999999</v>
+        <v>14.531919</v>
       </c>
       <c r="T3">
+        <v>14.970844999999999</v>
+      </c>
+      <c r="U3">
         <v>2.8411999999999997</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>2.9591500000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>192</v>
       </c>
@@ -13853,10 +13938,10 @@
         <v>2.3544</v>
       </c>
       <c r="F4" s="21">
-        <v>8.2236000000000011</v>
+        <v>8.6800315000000001</v>
       </c>
       <c r="G4" s="21">
-        <v>8.6032999999999991</v>
+        <v>9.0720564999999986</v>
       </c>
       <c r="H4" s="21">
         <v>2.1535500000000001</v>
@@ -13865,10 +13950,10 @@
         <v>2.3201499999999999</v>
       </c>
       <c r="J4" s="21">
-        <v>10.42825</v>
+        <v>10.867018499999997</v>
       </c>
       <c r="K4" s="21">
-        <v>10.841000000000006</v>
+        <v>11.292242500000008</v>
       </c>
       <c r="L4" s="21">
         <v>2.55335</v>
@@ -13876,32 +13961,36 @@
       <c r="M4" s="21">
         <v>2.6930500000000022</v>
       </c>
-      <c r="N4">
-        <v>8.5152000000000001</v>
+      <c r="N4" s="27">
+        <f t="shared" ref="N4:N9" si="0">1-L4/J4</f>
+        <v>0.76503674858011872</v>
       </c>
       <c r="O4">
-        <v>8.6844999999999999</v>
+        <v>8.9549250000000011</v>
       </c>
       <c r="P4">
+        <v>9.1351940000000003</v>
+      </c>
+      <c r="Q4">
         <v>2.2601999999999998</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>2.3608000000000002</v>
       </c>
-      <c r="R4" s="29">
-        <v>9.5402999999999984</v>
-      </c>
       <c r="S4" s="29">
-        <v>9.8483000000000001</v>
-      </c>
-      <c r="T4">
+        <v>9.9824789999999997</v>
+      </c>
+      <c r="T4" s="29">
+        <v>10.301406</v>
+      </c>
+      <c r="U4">
         <v>2.2308000000000003</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>2.3284000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>256</v>
       </c>
@@ -13918,10 +14007,10 @@
         <v>2.1312500000000001</v>
       </c>
       <c r="F5" s="21">
-        <v>5.8582000000000001</v>
+        <v>6.2979319999999994</v>
       </c>
       <c r="G5" s="21">
-        <v>5.9985499999999998</v>
+        <v>6.4558615000000001</v>
       </c>
       <c r="H5" s="21">
         <v>1.8953</v>
@@ -13930,10 +14019,10 @@
         <v>2.0604500000000003</v>
       </c>
       <c r="J5" s="21">
-        <v>7.3516000000000004</v>
+        <v>7.7882359999999995</v>
       </c>
       <c r="K5" s="21">
-        <v>7.5841500000000002</v>
+        <v>8.0273275000000019</v>
       </c>
       <c r="L5" s="21">
         <v>2.0696500000000002</v>
@@ -13941,32 +14030,36 @@
       <c r="M5" s="21">
         <v>2.2613000000000003</v>
       </c>
-      <c r="N5">
-        <v>6.3908500000000004</v>
+      <c r="N5" s="27">
+        <f t="shared" si="0"/>
+        <v>0.73425946517285812</v>
       </c>
       <c r="O5">
-        <v>6.5433999999999992</v>
+        <v>6.8351664999999997</v>
       </c>
       <c r="P5">
+        <v>6.9901595000000007</v>
+      </c>
+      <c r="Q5">
         <v>1.8931</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>1.94425</v>
       </c>
-      <c r="R5">
-        <v>7.1855500000000001</v>
-      </c>
       <c r="S5">
-        <v>7.5023000000000009</v>
+        <v>7.627080499999999</v>
       </c>
       <c r="T5">
+        <v>7.9521390000000007</v>
+      </c>
+      <c r="U5">
         <v>1.8946000000000001</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>1.9694</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>320</v>
       </c>
@@ -13983,10 +14076,10 @@
         <v>1.7584000000000002</v>
       </c>
       <c r="F6" s="21">
-        <v>4.8888999999999996</v>
+        <v>5.3486039999999999</v>
       </c>
       <c r="G6" s="21">
-        <v>5.0956999999999999</v>
+        <v>5.5564615000000002</v>
       </c>
       <c r="H6" s="21">
         <v>1.7514000000000001</v>
@@ -13995,10 +14088,10 @@
         <v>2.2029999999999998</v>
       </c>
       <c r="J6" s="21">
-        <v>6.0501000000000005</v>
+        <v>6.4936315000000011</v>
       </c>
       <c r="K6" s="21">
-        <v>6.695400000000002</v>
+        <v>7.1455015000000017</v>
       </c>
       <c r="L6" s="21">
         <v>1.9704000000000002</v>
@@ -14006,32 +14099,36 @@
       <c r="M6" s="21">
         <v>2.2710000000000021</v>
       </c>
-      <c r="N6">
-        <v>5.0598000000000001</v>
+      <c r="N6" s="27">
+        <f t="shared" si="0"/>
+        <v>0.69656424144178808</v>
       </c>
       <c r="O6">
-        <v>5.2791000000000006</v>
+        <v>5.5005895000000002</v>
       </c>
       <c r="P6">
+        <v>5.7364354999999998</v>
+      </c>
+      <c r="Q6">
         <v>1.7212499999999999</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1.82955</v>
       </c>
-      <c r="R6">
-        <v>5.6292999999999997</v>
-      </c>
       <c r="S6">
-        <v>5.8271000000000015</v>
+        <v>6.0706370000000005</v>
       </c>
       <c r="T6">
+        <v>6.2845350000000009</v>
+      </c>
+      <c r="U6">
         <v>1.6910499999999999</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>1.7534000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>384</v>
       </c>
@@ -14048,10 +14145,10 @@
         <v>1.7197</v>
       </c>
       <c r="F7" s="21">
-        <v>3.9879499999999997</v>
+        <v>4.4421464999999998</v>
       </c>
       <c r="G7" s="21">
-        <v>4.0850499999999998</v>
+        <v>4.5426000000000002</v>
       </c>
       <c r="H7" s="21">
         <v>1.6086500000000001</v>
@@ -14060,10 +14157,10 @@
         <v>1.7222500000000001</v>
       </c>
       <c r="J7" s="21">
-        <v>4.7641999999999998</v>
+        <v>5.2042145000000009</v>
       </c>
       <c r="K7" s="21">
-        <v>4.8965500000000004</v>
+        <v>5.3488220000000002</v>
       </c>
       <c r="L7" s="21">
         <v>1.67875</v>
@@ -14071,32 +14168,36 @@
       <c r="M7" s="21">
         <v>1.7477000000000003</v>
       </c>
-      <c r="N7">
-        <v>4.1367500000000001</v>
+      <c r="N7" s="27">
+        <f t="shared" si="0"/>
+        <v>0.67742490245165721</v>
       </c>
       <c r="O7">
-        <v>4.2753500000000004</v>
+        <v>4.5758350000000005</v>
       </c>
       <c r="P7">
+        <v>4.7254869999999993</v>
+      </c>
+      <c r="Q7">
         <v>1.6033499999999998</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>1.6649500000000002</v>
       </c>
-      <c r="R7">
-        <v>4.5728999999999997</v>
-      </c>
       <c r="S7">
-        <v>4.7068500000000002</v>
+        <v>5.0136354999999986</v>
       </c>
       <c r="T7">
+        <v>5.1528295000000002</v>
+      </c>
+      <c r="U7">
         <v>1.5882499999999999</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>1.6602000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>448</v>
       </c>
@@ -14113,10 +14214,10 @@
         <v>1.5283</v>
       </c>
       <c r="F8" s="21">
-        <v>3.39845</v>
+        <v>3.8551370000000009</v>
       </c>
       <c r="G8" s="21">
-        <v>3.4793499999999997</v>
+        <v>3.9505850000000002</v>
       </c>
       <c r="H8" s="21">
         <v>1.56555</v>
@@ -14125,10 +14226,10 @@
         <v>1.7153</v>
       </c>
       <c r="J8" s="21">
-        <v>4.06175</v>
+        <v>4.5009115000000008</v>
       </c>
       <c r="K8" s="21">
-        <v>4.2613000000000003</v>
+        <v>4.7084974999999991</v>
       </c>
       <c r="L8" s="21">
         <v>1.5960000000000001</v>
@@ -14136,32 +14237,36 @@
       <c r="M8" s="21">
         <v>1.7636500000000002</v>
       </c>
-      <c r="N8">
-        <v>3.5381</v>
+      <c r="N8" s="27">
+        <f t="shared" si="0"/>
+        <v>0.64540515848845281</v>
       </c>
       <c r="O8">
-        <v>3.6567500000000002</v>
+        <v>3.9798525000000007</v>
       </c>
       <c r="P8">
+        <v>4.1028959999999994</v>
+      </c>
+      <c r="Q8">
         <v>1.5258</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>1.5828</v>
       </c>
-      <c r="R8">
-        <v>3.9009499999999999</v>
-      </c>
       <c r="S8">
-        <v>4.0278</v>
+        <v>4.3454945</v>
       </c>
       <c r="T8">
+        <v>4.4759270000000004</v>
+      </c>
+      <c r="U8">
         <v>1.5144500000000001</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1.5534000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>512</v>
       </c>
@@ -14178,10 +14283,10 @@
         <v>1.6849999999999998</v>
       </c>
       <c r="F9" s="21">
-        <v>2.9441999999999999</v>
+        <v>3.4013584999999997</v>
       </c>
       <c r="G9" s="21">
-        <v>3.0791500000000003</v>
+        <v>3.5665500000000003</v>
       </c>
       <c r="H9" s="21">
         <v>1.5003499999999999</v>
@@ -14190,10 +14295,10 @@
         <v>1.6402000000000001</v>
       </c>
       <c r="J9" s="21">
-        <v>3.5368000000000004</v>
+        <v>3.9799080000000009</v>
       </c>
       <c r="K9" s="21">
-        <v>3.6219999999999999</v>
+        <v>4.0680405000000004</v>
       </c>
       <c r="L9" s="21">
         <v>1.5340597014925372</v>
@@ -14201,140 +14306,154 @@
       <c r="M9" s="21">
         <v>1.6802999999999997</v>
       </c>
-      <c r="N9">
-        <v>3.0644499999999999</v>
+      <c r="N9" s="27">
+        <f t="shared" si="0"/>
+        <v>0.61454895402292298</v>
       </c>
       <c r="O9">
-        <v>3.1629999999999998</v>
+        <v>3.5054605000000003</v>
       </c>
       <c r="P9">
+        <v>3.6048149999999999</v>
+      </c>
+      <c r="Q9">
         <v>1.46055</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>1.5424500000000001</v>
       </c>
-      <c r="R9">
-        <v>3.3694499999999996</v>
-      </c>
       <c r="S9">
-        <v>3.4679000000000002</v>
+        <v>3.8091395000000001</v>
       </c>
       <c r="T9">
+        <v>3.9268395000000003</v>
+      </c>
+      <c r="U9">
         <v>1.4807999999999999</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>1.5562</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S19">
+        <f t="shared" ref="S19:T19" si="1">S10/1000</f>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
       <c r="B46" s="2"/>
-      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="23"/>
       <c r="B47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P48" s="2"/>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P49" s="22"/>
+    <row r="49" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q49" s="22"/>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P50" s="23"/>
+    <row r="50" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14343,11 +14462,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DE693F-DFBF-A645-98AD-B3E2E7E6F16B}">
-  <dimension ref="A1:AE48"/>
+  <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="113" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG21" sqref="AG21:AH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14356,67 +14475,76 @@
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42"/>
+      <c r="E1" s="55"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47" t="s">
+      <c r="H1" s="49"/>
+      <c r="I1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="47"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="30"/>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="50"/>
-      <c r="N1" s="51" t="s">
+      <c r="M1" s="63"/>
+      <c r="N1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="51"/>
+      <c r="O1" s="64"/>
       <c r="P1" s="32"/>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="52"/>
-      <c r="S1" s="53" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="53"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="54" t="s">
+      <c r="T1" s="60"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55" t="s">
+      <c r="W1" s="61"/>
+      <c r="X1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="43" t="s">
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="44" t="s">
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="60"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="38"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" s="54"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14507,8 +14635,23 @@
       <c r="AE2" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="AF2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>128</v>
       </c>
@@ -14524,7 +14667,7 @@
       <c r="E3" s="21">
         <v>519.1</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="67">
         <f>1-D3/B3</f>
         <v>5.5833934022036735E-2</v>
       </c>
@@ -14540,7 +14683,7 @@
       <c r="J3" s="21">
         <v>771.30000000000007</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="67">
         <f>1-I3/G3</f>
         <v>6.2411719344502403E-2</v>
       </c>
@@ -14556,7 +14699,7 @@
       <c r="O3">
         <v>1145.5500000000002</v>
       </c>
-      <c r="P3" s="27">
+      <c r="P3" s="67">
         <f>1-N3/L3</f>
         <v>0.21016725493084965</v>
       </c>
@@ -14572,7 +14715,7 @@
       <c r="T3">
         <v>696.05000000000007</v>
       </c>
-      <c r="U3" s="27">
+      <c r="U3" s="67">
         <f>1-S3/Q3</f>
         <v>0.38039275930050953</v>
       </c>
@@ -14588,28 +14731,44 @@
       <c r="Y3">
         <v>5841.7</v>
       </c>
-      <c r="Z3" s="27">
+      <c r="Z3" s="67">
         <f>1-X3/V3</f>
         <v>0.14793472775325645</v>
       </c>
-      <c r="AA3" s="21">
+      <c r="AA3" s="68">
         <v>12584.279</v>
       </c>
-      <c r="AB3" s="21">
+      <c r="AB3" s="68">
         <v>12847.5445</v>
       </c>
-      <c r="AC3" s="21">
+      <c r="AC3" s="68">
         <v>2763.55</v>
       </c>
-      <c r="AD3" s="21">
+      <c r="AD3" s="68">
         <v>3719.4500000000003</v>
       </c>
-      <c r="AE3" s="27">
+      <c r="AE3" s="67">
         <f>1-AC3/AA3</f>
         <v>0.78039663615213872</v>
       </c>
+      <c r="AF3">
+        <v>644.81949999999995</v>
+      </c>
+      <c r="AG3">
+        <v>670.36799999999994</v>
+      </c>
+      <c r="AH3">
+        <v>704.9</v>
+      </c>
+      <c r="AI3">
+        <v>726.55</v>
+      </c>
+      <c r="AJ3" s="67">
+        <f t="shared" ref="AJ3:AJ8" si="0">1-AH3/AF3</f>
+        <v>-9.3174136328073365E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>192</v>
       </c>
@@ -14625,8 +14784,8 @@
       <c r="E4" s="21">
         <v>398.1</v>
       </c>
-      <c r="F4" s="27">
-        <f t="shared" ref="F4:F9" si="0">1-D4/B4</f>
+      <c r="F4" s="67">
+        <f t="shared" ref="F4:F9" si="1">1-D4/B4</f>
         <v>2.6579607416876594E-2</v>
       </c>
       <c r="G4" s="21">
@@ -14641,8 +14800,8 @@
       <c r="J4" s="21">
         <v>649.15</v>
       </c>
-      <c r="K4" s="27">
-        <f t="shared" ref="K4:K9" si="1">1-I4/G4</f>
+      <c r="K4" s="67">
+        <f t="shared" ref="K4:K9" si="2">1-I4/G4</f>
         <v>6.1931890775252851E-2</v>
       </c>
       <c r="L4">
@@ -14657,8 +14816,8 @@
       <c r="O4">
         <v>913.00000000000011</v>
       </c>
-      <c r="P4" s="27">
-        <f t="shared" ref="P4:P9" si="2">1-N4/L4</f>
+      <c r="P4" s="67">
+        <f t="shared" ref="P4:P9" si="3">1-N4/L4</f>
         <v>0.19360501055261359</v>
       </c>
       <c r="Q4">
@@ -14673,8 +14832,8 @@
       <c r="T4">
         <v>587.75</v>
       </c>
-      <c r="U4" s="27">
-        <f t="shared" ref="U4:U9" si="3">1-S4/Q4</f>
+      <c r="U4" s="67">
+        <f t="shared" ref="U4:U9" si="4">1-S4/Q4</f>
         <v>0.35172752844815802</v>
       </c>
       <c r="V4">
@@ -14689,28 +14848,44 @@
       <c r="Y4">
         <v>4203.9500000000007</v>
       </c>
-      <c r="Z4" s="27">
-        <f t="shared" ref="Z4:Z9" si="4">1-X4/V4</f>
+      <c r="Z4" s="67">
+        <f t="shared" ref="Z4:Z9" si="5">1-X4/V4</f>
         <v>0.13277589431743808</v>
       </c>
-      <c r="AA4" s="21">
+      <c r="AA4" s="68">
         <v>8680.031500000001</v>
       </c>
-      <c r="AB4" s="21">
+      <c r="AB4" s="68">
         <v>9072.0564999999988</v>
       </c>
-      <c r="AC4" s="21">
+      <c r="AC4" s="68">
         <v>2153.5500000000002</v>
       </c>
-      <c r="AD4" s="21">
+      <c r="AD4" s="68">
         <v>2320.15</v>
       </c>
-      <c r="AE4" s="27">
-        <f t="shared" ref="AE4:AE9" si="5">1-AC4/AA4</f>
+      <c r="AE4" s="67">
+        <f t="shared" ref="AE4:AE9" si="6">1-AC4/AA4</f>
         <v>0.7518960616675181</v>
       </c>
+      <c r="AF4">
+        <v>463.63500000000005</v>
+      </c>
+      <c r="AG4">
+        <v>478.06750000000005</v>
+      </c>
+      <c r="AH4">
+        <v>522.5</v>
+      </c>
+      <c r="AI4">
+        <v>545.04999999999995</v>
+      </c>
+      <c r="AJ4" s="67">
+        <f t="shared" si="0"/>
+        <v>-0.12696409891401639</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>256</v>
       </c>
@@ -14726,8 +14901,8 @@
       <c r="E5" s="21">
         <v>376.90000000000015</v>
       </c>
-      <c r="F5" s="27">
-        <f t="shared" si="0"/>
+      <c r="F5" s="67">
+        <f t="shared" si="1"/>
         <v>-7.9280134913822131E-2</v>
       </c>
       <c r="G5" s="21">
@@ -14742,8 +14917,8 @@
       <c r="J5" s="21">
         <v>588.15000000000009</v>
       </c>
-      <c r="K5" s="27">
-        <f t="shared" si="1"/>
+      <c r="K5" s="67">
+        <f t="shared" si="2"/>
         <v>6.8002842663328344E-2</v>
       </c>
       <c r="L5">
@@ -14758,8 +14933,8 @@
       <c r="O5">
         <v>901.05000000000007</v>
       </c>
-      <c r="P5" s="27">
-        <f t="shared" si="2"/>
+      <c r="P5" s="67">
+        <f t="shared" si="3"/>
         <v>0.18418994717230208</v>
       </c>
       <c r="Q5">
@@ -14774,8 +14949,8 @@
       <c r="T5">
         <v>549</v>
       </c>
-      <c r="U5" s="27">
-        <f t="shared" si="3"/>
+      <c r="U5" s="67">
+        <f t="shared" si="4"/>
         <v>0.3234057044223313</v>
       </c>
       <c r="V5">
@@ -14790,28 +14965,44 @@
       <c r="Y5">
         <v>3125</v>
       </c>
-      <c r="Z5" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z5" s="67">
+        <f t="shared" si="5"/>
         <v>0.14634669477451423</v>
       </c>
-      <c r="AA5" s="21">
+      <c r="AA5" s="68">
         <v>6297.9319999999998</v>
       </c>
-      <c r="AB5" s="21">
+      <c r="AB5" s="68">
         <v>6455.8615</v>
       </c>
-      <c r="AC5" s="21">
+      <c r="AC5" s="68">
         <v>1895.3</v>
       </c>
-      <c r="AD5" s="21">
+      <c r="AD5" s="68">
         <v>2060.4500000000003</v>
       </c>
-      <c r="AE5" s="27">
-        <f t="shared" si="5"/>
+      <c r="AE5" s="67">
+        <f t="shared" si="6"/>
         <v>0.69905994539159844</v>
       </c>
+      <c r="AF5">
+        <v>365.346</v>
+      </c>
+      <c r="AG5">
+        <v>375.68349999999998</v>
+      </c>
+      <c r="AH5" s="40">
+        <v>426.25</v>
+      </c>
+      <c r="AI5" s="39">
+        <v>432.3</v>
+      </c>
+      <c r="AJ5" s="67">
+        <f t="shared" si="0"/>
+        <v>-0.16670224937456557</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>320</v>
       </c>
@@ -14827,8 +15018,8 @@
       <c r="E6" s="21">
         <v>310.35000000000002</v>
       </c>
-      <c r="F6" s="27">
-        <f t="shared" si="0"/>
+      <c r="F6" s="67">
+        <f t="shared" si="1"/>
         <v>-3.8883380787015254E-2</v>
       </c>
       <c r="G6" s="21">
@@ -14843,8 +15034,8 @@
       <c r="J6" s="21">
         <v>692.80000000000007</v>
       </c>
-      <c r="K6" s="27">
-        <f t="shared" si="1"/>
+      <c r="K6" s="67">
+        <f t="shared" si="2"/>
         <v>1.7048549794708157E-2</v>
       </c>
       <c r="L6">
@@ -14859,8 +15050,8 @@
       <c r="O6">
         <v>881.3</v>
       </c>
-      <c r="P6" s="27">
-        <f t="shared" si="2"/>
+      <c r="P6" s="67">
+        <f t="shared" si="3"/>
         <v>0.18707655305307913</v>
       </c>
       <c r="Q6">
@@ -14875,8 +15066,8 @@
       <c r="T6">
         <v>521.29999999999995</v>
       </c>
-      <c r="U6" s="27">
-        <f t="shared" si="3"/>
+      <c r="U6" s="67">
+        <f t="shared" si="4"/>
         <v>0.30116463299856</v>
       </c>
       <c r="V6">
@@ -14891,28 +15082,44 @@
       <c r="Y6">
         <v>2613.4</v>
       </c>
-      <c r="Z6" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z6" s="67">
+        <f t="shared" si="5"/>
         <v>0.14880437199408048</v>
       </c>
-      <c r="AA6" s="21">
+      <c r="AA6" s="68">
         <v>5348.6040000000003</v>
       </c>
-      <c r="AB6" s="21">
+      <c r="AB6" s="68">
         <v>5556.4615000000003</v>
       </c>
-      <c r="AC6" s="21">
+      <c r="AC6" s="68">
         <v>1751.4</v>
       </c>
-      <c r="AD6" s="21">
+      <c r="AD6" s="68">
         <v>2203</v>
       </c>
-      <c r="AE6" s="27">
-        <f t="shared" si="5"/>
+      <c r="AE6" s="67">
+        <f t="shared" si="6"/>
         <v>0.67255007100918296</v>
       </c>
+      <c r="AF6">
+        <v>321.17699999999991</v>
+      </c>
+      <c r="AG6">
+        <v>334.2165</v>
+      </c>
+      <c r="AH6" s="29">
+        <v>378.5</v>
+      </c>
+      <c r="AI6" s="29">
+        <v>393.05</v>
+      </c>
+      <c r="AJ6" s="67">
+        <f t="shared" si="0"/>
+        <v>-0.1784779109338468</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>384</v>
       </c>
@@ -14928,8 +15135,8 @@
       <c r="E7" s="21">
         <v>314.25000000000006</v>
       </c>
-      <c r="F7" s="27">
-        <f t="shared" si="0"/>
+      <c r="F7" s="67">
+        <f t="shared" si="1"/>
         <v>-0.13318749591514267</v>
       </c>
       <c r="G7" s="21">
@@ -14944,8 +15151,8 @@
       <c r="J7" s="21">
         <v>668.45</v>
       </c>
-      <c r="K7" s="27">
-        <f t="shared" si="1"/>
+      <c r="K7" s="67">
+        <f t="shared" si="2"/>
         <v>4.2218045435103102E-2</v>
       </c>
       <c r="L7">
@@ -14960,8 +15167,8 @@
       <c r="O7">
         <v>903.80000000000007</v>
       </c>
-      <c r="P7" s="27">
-        <f t="shared" si="2"/>
+      <c r="P7" s="67">
+        <f t="shared" si="3"/>
         <v>0.17635508311291204</v>
       </c>
       <c r="Q7">
@@ -14976,8 +15183,8 @@
       <c r="T7">
         <v>512.25</v>
       </c>
-      <c r="U7" s="27">
-        <f t="shared" si="3"/>
+      <c r="U7" s="67">
+        <f t="shared" si="4"/>
         <v>0.2768007822509152</v>
       </c>
       <c r="V7">
@@ -14992,28 +15199,44 @@
       <c r="Y7">
         <v>2260.6</v>
       </c>
-      <c r="Z7" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z7" s="67">
+        <f t="shared" si="5"/>
         <v>0.15546448573519356</v>
       </c>
-      <c r="AA7" s="21">
+      <c r="AA7" s="68">
         <v>4442.1464999999998</v>
       </c>
-      <c r="AB7" s="21">
+      <c r="AB7" s="68">
         <v>4542.6000000000004</v>
       </c>
-      <c r="AC7" s="21">
+      <c r="AC7" s="68">
         <v>1608.65</v>
       </c>
-      <c r="AD7" s="21">
+      <c r="AD7" s="68">
         <v>1722.25</v>
       </c>
-      <c r="AE7" s="27">
-        <f t="shared" si="5"/>
+      <c r="AE7" s="67">
+        <f t="shared" si="6"/>
         <v>0.63786651340742584</v>
       </c>
+      <c r="AF7">
+        <v>292.59100000000007</v>
+      </c>
+      <c r="AG7">
+        <v>303.55800000000005</v>
+      </c>
+      <c r="AH7" s="29">
+        <v>356.2</v>
+      </c>
+      <c r="AI7" s="29">
+        <v>374.50000000000017</v>
+      </c>
+      <c r="AJ7" s="67">
+        <f t="shared" si="0"/>
+        <v>-0.21739903141244921</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>448</v>
       </c>
@@ -15029,8 +15252,8 @@
       <c r="E8" s="21">
         <v>310.30000000000013</v>
       </c>
-      <c r="F8" s="27">
-        <f t="shared" si="0"/>
+      <c r="F8" s="67">
+        <f t="shared" si="1"/>
         <v>-0.14232110718782964</v>
       </c>
       <c r="G8" s="21">
@@ -15045,8 +15268,8 @@
       <c r="J8" s="21">
         <v>657.8</v>
       </c>
-      <c r="K8" s="27">
-        <f t="shared" si="1"/>
+      <c r="K8" s="67">
+        <f t="shared" si="2"/>
         <v>3.0868132930943148E-2</v>
       </c>
       <c r="L8">
@@ -15061,8 +15284,8 @@
       <c r="O8">
         <v>908.10000000000014</v>
       </c>
-      <c r="P8" s="27">
-        <f t="shared" si="2"/>
+      <c r="P8" s="67">
+        <f t="shared" si="3"/>
         <v>0.17465441862189512</v>
       </c>
       <c r="Q8">
@@ -15077,8 +15300,8 @@
       <c r="T8">
         <v>501.1</v>
       </c>
-      <c r="U8" s="27">
-        <f t="shared" si="3"/>
+      <c r="U8" s="67">
+        <f t="shared" si="4"/>
         <v>0.2520008800907555</v>
       </c>
       <c r="V8">
@@ -15093,28 +15316,44 @@
       <c r="Y8">
         <v>2013.9</v>
       </c>
-      <c r="Z8" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z8" s="67">
+        <f t="shared" si="5"/>
         <v>0.15739746637150331</v>
       </c>
-      <c r="AA8" s="21">
+      <c r="AA8" s="68">
         <v>3855.1370000000011</v>
       </c>
-      <c r="AB8" s="21">
+      <c r="AB8" s="68">
         <v>3950.585</v>
       </c>
-      <c r="AC8" s="21">
+      <c r="AC8" s="68">
         <v>1565.55</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AD8" s="68">
         <v>1715.3</v>
       </c>
-      <c r="AE8" s="27">
-        <f t="shared" si="5"/>
+      <c r="AE8" s="67">
+        <f t="shared" si="6"/>
         <v>0.59390548247701713</v>
       </c>
+      <c r="AF8">
+        <v>253.21549999999996</v>
+      </c>
+      <c r="AG8">
+        <v>262.685</v>
+      </c>
+      <c r="AH8">
+        <v>318.3</v>
+      </c>
+      <c r="AI8">
+        <v>329.25000000000006</v>
+      </c>
+      <c r="AJ8" s="67">
+        <f t="shared" si="0"/>
+        <v>-0.2570320537249895</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>512</v>
       </c>
@@ -15130,8 +15369,8 @@
       <c r="E9" s="21">
         <v>277.3</v>
       </c>
-      <c r="F9" s="27">
-        <f t="shared" si="0"/>
+      <c r="F9" s="67">
+        <f t="shared" si="1"/>
         <v>-0.1277446801298292</v>
       </c>
       <c r="G9" s="21">
@@ -15146,8 +15385,8 @@
       <c r="J9" s="21">
         <v>571.85</v>
       </c>
-      <c r="K9" s="27">
-        <f t="shared" si="1"/>
+      <c r="K9" s="67">
+        <f t="shared" si="2"/>
         <v>4.3051411386417437E-2</v>
       </c>
       <c r="L9">
@@ -15162,8 +15401,8 @@
       <c r="O9">
         <v>883.9</v>
       </c>
-      <c r="P9" s="27">
-        <f t="shared" si="2"/>
+      <c r="P9" s="67">
+        <f t="shared" si="3"/>
         <v>0.18331991640071821</v>
       </c>
       <c r="Q9">
@@ -15178,8 +15417,8 @@
       <c r="T9">
         <v>489.15</v>
       </c>
-      <c r="U9" s="27">
-        <f t="shared" si="3"/>
+      <c r="U9" s="67">
+        <f t="shared" si="4"/>
         <v>0.24972109110278617</v>
       </c>
       <c r="V9">
@@ -15194,54 +15433,255 @@
       <c r="Y9">
         <v>1848.95</v>
       </c>
-      <c r="Z9" s="27">
-        <f t="shared" si="4"/>
+      <c r="Z9" s="67">
+        <f t="shared" si="5"/>
         <v>0.13742937220313645</v>
       </c>
-      <c r="AA9" s="21">
+      <c r="AA9" s="68">
         <v>3401.3584999999998</v>
       </c>
-      <c r="AB9" s="21">
+      <c r="AB9" s="68">
         <v>3566.55</v>
       </c>
-      <c r="AC9" s="21">
+      <c r="AC9" s="68">
         <v>1500.35</v>
       </c>
-      <c r="AD9" s="21">
+      <c r="AD9" s="68">
         <v>1640.2</v>
       </c>
-      <c r="AE9" s="27">
-        <f t="shared" si="5"/>
+      <c r="AE9" s="67">
+        <f t="shared" si="6"/>
         <v>0.55889683489699782</v>
       </c>
+      <c r="AF9">
+        <v>234.52199999999999</v>
+      </c>
+      <c r="AG9">
+        <v>249.9975</v>
+      </c>
+      <c r="AH9">
+        <v>299.5</v>
+      </c>
+      <c r="AI9">
+        <v>310.65000000000003</v>
+      </c>
+      <c r="AJ9" s="67">
+        <f>1-AH9/AF9</f>
+        <v>-0.27706569106523049</v>
+      </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="56"/>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>576</v>
+      </c>
+      <c r="AA10" s="68">
+        <v>2967.4119999999994</v>
+      </c>
+      <c r="AB10" s="68">
+        <v>3068.2339999999999</v>
+      </c>
+      <c r="AC10" s="68">
+        <v>1418.15</v>
+      </c>
+      <c r="AD10" s="68">
+        <v>1532.65</v>
+      </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>640</v>
+      </c>
+      <c r="AA11" s="68">
+        <v>2704.2674999999995</v>
+      </c>
+      <c r="AB11" s="68">
+        <v>2794.0855000000001</v>
+      </c>
+      <c r="AC11" s="68">
+        <v>1345.65</v>
+      </c>
+      <c r="AD11" s="68">
+        <v>1423.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>704</v>
+      </c>
+      <c r="AA12" s="68">
+        <v>2488.4484999999995</v>
+      </c>
+      <c r="AB12" s="68">
+        <v>2597.2195000000002</v>
+      </c>
+      <c r="AC12" s="68">
+        <v>1453</v>
+      </c>
+      <c r="AD12" s="68">
+        <v>1539.7500000000016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>768</v>
+      </c>
+      <c r="AA13" s="68">
+        <v>2297.357</v>
+      </c>
+      <c r="AB13" s="68">
+        <v>2346.4409999999998</v>
+      </c>
+      <c r="AC13" s="68">
+        <v>1332.8</v>
+      </c>
+      <c r="AD13" s="68">
+        <v>1407.0500000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>832</v>
+      </c>
+      <c r="AA14" s="68">
+        <v>2175.2925</v>
+      </c>
+      <c r="AB14" s="68">
+        <v>2235.64</v>
+      </c>
+      <c r="AC14" s="68">
+        <v>1332.45</v>
+      </c>
+      <c r="AD14" s="68">
+        <v>1396.1000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>896</v>
+      </c>
+      <c r="AA15" s="68">
+        <v>2038.9569999999999</v>
+      </c>
+      <c r="AB15" s="68">
+        <v>2099.6795000000002</v>
+      </c>
+      <c r="AC15" s="68">
+        <v>1295.25</v>
+      </c>
+      <c r="AD15" s="68">
+        <v>1339.3500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>960</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="33"/>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="69">
+        <v>1944.2395000000001</v>
+      </c>
+      <c r="AB16" s="69">
+        <v>1997.9580000000001</v>
+      </c>
+      <c r="AC16" s="68">
+        <v>1329.0526315789473</v>
+      </c>
+      <c r="AD16" s="68">
+        <v>1609.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>1024</v>
+      </c>
+      <c r="Q17">
+        <v>14</v>
+      </c>
+      <c r="AA17" s="69">
+        <v>1852.7779999999996</v>
+      </c>
+      <c r="AB17" s="69">
+        <v>1926.6369999999999</v>
+      </c>
+      <c r="AC17" s="68">
+        <v>1275.4000000000001</v>
+      </c>
+      <c r="AD17" s="68">
+        <v>1340.7500000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>2048</v>
+      </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="27"/>
+      <c r="Q18">
+        <v>64</v>
+      </c>
+      <c r="AA18" s="68">
+        <v>1250.7869999999998</v>
+      </c>
+      <c r="AB18" s="68">
+        <v>1288.0135</v>
+      </c>
+      <c r="AC18" s="68">
+        <v>1245.5999999999999</v>
+      </c>
+      <c r="AD18" s="68">
+        <v>1429.6000000000001</v>
+      </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>3008</v>
+      </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="27"/>
+      <c r="Q19">
+        <v>83</v>
+      </c>
+      <c r="AA19" s="68">
+        <v>1205.6444999999999</v>
+      </c>
+      <c r="AB19" s="68">
+        <v>1236.9480000000001</v>
+      </c>
+      <c r="AC19" s="70">
+        <v>1194.7142857142858</v>
+      </c>
+      <c r="AD19" s="70">
+        <v>1251.3999999999999</v>
+      </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G20" s="27"/>
+      <c r="Q20">
+        <v>126</v>
+      </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G21" s="27"/>
+      <c r="Q21">
+        <v>186</v>
+      </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G22" s="27"/>
+      <c r="Q22">
+        <v>230</v>
+      </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
@@ -15324,23 +15764,26 @@
       <c r="B48" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -15349,8 +15792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C7387A-1CBC-9545-9516-2C253950AE23}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="172" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15359,21 +15802,21 @@
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42"/>
+      <c r="E1" s="55"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="54"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -15387,7 +15830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>128</v>
       </c>
@@ -15404,7 +15847,7 @@
         <v>2.9409999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>192</v>
       </c>
@@ -15421,7 +15864,7 @@
         <v>2.3544</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>256</v>
       </c>
@@ -15438,7 +15881,7 @@
         <v>2.1312500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>320</v>
       </c>
@@ -15455,7 +15898,7 @@
         <v>1.7584000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>384</v>
       </c>
@@ -15472,7 +15915,7 @@
         <v>1.7197</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>448</v>
       </c>
@@ -15488,12 +15931,8 @@
       <c r="E8" s="21">
         <v>1.5283</v>
       </c>
-      <c r="H8">
-        <f>B3/D3</f>
-        <v>4.8044465163841972</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>512</v>
       </c>
@@ -15509,12 +15948,8 @@
       <c r="E9" s="21">
         <v>1.6849999999999998</v>
       </c>
-      <c r="H9">
-        <f>B4/D4</f>
-        <v>4.0937753538267385</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>1024</v>
       </c>
@@ -15530,12 +15965,8 @@
       <c r="E10" s="21">
         <v>1.6154999999999997</v>
       </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H13" si="0">B5/D5</f>
-        <v>3.5125857080227973</v>
-      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>1536</v>
       </c>
@@ -15551,12 +15982,8 @@
       <c r="E11" s="21">
         <v>1.4418499999999999</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>3.1599732900887152</v>
-      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>2048</v>
       </c>
@@ -15572,12 +15999,8 @@
       <c r="E12" s="21">
         <v>1.4190999999999998</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>2.8050819547538826</v>
-      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>2560</v>
       </c>
@@ -15593,13 +16016,9 @@
       <c r="E13" s="21">
         <v>1.6719999999999999</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>2.5092482672614338</v>
-      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>3008</v>
       </c>
       <c r="B14" s="26">
@@ -15613,24 +16032,6 @@
       </c>
       <c r="E14" s="21">
         <v>1.4667999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E18">
-        <f>D3/D14</f>
-        <v>2.3813604751806694</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C20">
-        <f>B3/B14</f>
-        <v>14.372403368602892</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C26">
-        <f>C20-E18</f>
-        <v>11.991042893422224</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -15657,7 +16058,7 @@
         <v>9082.4500000000007</v>
       </c>
       <c r="R40">
-        <f t="shared" ref="R40:R50" si="1">Q40/1000</f>
+        <f t="shared" ref="R40:R50" si="0">Q40/1000</f>
         <v>9.0824500000000015</v>
       </c>
     </row>
@@ -15669,14 +16070,14 @@
         <v>2.7707083333333333</v>
       </c>
       <c r="P41">
-        <f t="shared" ref="P41:P51" si="2">B42/1000</f>
+        <f t="shared" ref="P41:P51" si="1">B42/1000</f>
         <v>2.2185999999999998E-3</v>
       </c>
       <c r="Q41" s="2">
         <v>6676.84</v>
       </c>
       <c r="R41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.6768400000000003</v>
       </c>
     </row>
@@ -15688,14 +16089,14 @@
         <v>2.2185999999999999</v>
       </c>
       <c r="P42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9008333333333332E-3</v>
       </c>
       <c r="Q42" s="2">
         <v>5300.16</v>
       </c>
       <c r="R42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.30016</v>
       </c>
     </row>
@@ -15707,14 +16108,14 @@
         <v>1.9008333333333332</v>
       </c>
       <c r="P43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.67728E-3</v>
       </c>
       <c r="Q43" s="2">
         <v>4429</v>
       </c>
       <c r="R43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.4290000000000003</v>
       </c>
     </row>
@@ -15726,14 +16127,14 @@
         <v>1.6772799999999999</v>
       </c>
       <c r="P44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5789200000000001E-3</v>
       </c>
       <c r="Q44" s="2">
         <v>3720.1111111111113</v>
       </c>
       <c r="R44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.7201111111111111</v>
       </c>
     </row>
@@ -15745,14 +16146,14 @@
         <v>1.5789200000000001</v>
       </c>
       <c r="P45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.48256E-3</v>
       </c>
       <c r="Q45" s="2">
         <v>3201.7</v>
       </c>
       <c r="R45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.2016999999999998</v>
       </c>
     </row>
@@ -15764,14 +16165,14 @@
         <v>1.4825599999999999</v>
       </c>
       <c r="P46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4725652173913043E-3</v>
       </c>
       <c r="Q46" s="2">
         <v>1577.909090909091</v>
       </c>
       <c r="R46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5779090909090909</v>
       </c>
     </row>
@@ -15783,14 +16184,14 @@
         <v>1.4725652173913042</v>
       </c>
       <c r="P47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3879090909090909E-3</v>
       </c>
       <c r="Q47" s="2">
         <v>1778.35</v>
       </c>
       <c r="R47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.7783499999999999</v>
       </c>
     </row>
@@ -15802,14 +16203,14 @@
         <v>1.387909090909091</v>
       </c>
       <c r="P48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.2533181818181818E-3</v>
       </c>
       <c r="Q48" s="2">
         <v>944.52</v>
       </c>
       <c r="R48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.94452000000000003</v>
       </c>
     </row>
@@ -15821,14 +16222,14 @@
         <v>1.2533181818181818</v>
       </c>
       <c r="P49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3562400000000001E-3</v>
       </c>
       <c r="Q49" s="22">
         <v>928.16666666666663</v>
       </c>
       <c r="R49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92816666666666658</v>
       </c>
     </row>
@@ -15840,14 +16241,14 @@
         <v>1.3562400000000001</v>
       </c>
       <c r="P50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3615833333333334E-3</v>
       </c>
       <c r="Q50" s="23">
         <v>926.2</v>
       </c>
       <c r="R50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92620000000000002</v>
       </c>
     </row>
@@ -15859,7 +16260,7 @@
         <v>1.3615833333333334</v>
       </c>
       <c r="P51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1634980769230769E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tests and analysis for paper 1
</commit_message>
<xml_diff>
--- a/experiments/lambda/analysis_run_cold.xlsx
+++ b/experiments/lambda/analysis_run_cold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimedantas/Documents/git/serverless-iot-deployment/experiments/lambda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7E83C9-2BC6-1645-A3D6-AC379247C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28C9D70-E1B0-AA49-B604-E59F8EF3FA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
   </bookViews>
   <sheets>
     <sheet name="run time" sheetId="2" r:id="rId1"/>
@@ -370,6 +370,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -448,10 +452,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1787,28 +1787,28 @@
             <c:numRef>
               <c:f>'cold start'!$C$3:$C$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.792399999999999</c:v>
+                  <c:v>14.136735999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1213300000000004</c:v>
+                  <c:v>9.9106820000000013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8608000000000002</c:v>
+                  <c:v>7.4673034999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5291000000000006</c:v>
+                  <c:v>6.0505819999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5209999999999999</c:v>
+                  <c:v>5.069757000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7754000000000003</c:v>
+                  <c:v>4.2812825000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2849499999999998</c:v>
+                  <c:v>3.8307094999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1885,7 +1885,7 @@
             <c:numRef>
               <c:f>'cold start'!$E$3:$E$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.9409999999999998</c:v>
@@ -2113,7 +2113,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2328,7 +2328,7 @@
             <c:numRef>
               <c:f>'cold start'!$H$3:$H$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.7635500000000004</c:v>
@@ -2434,7 +2434,7 @@
             <c:numRef>
               <c:f>'cold start'!$D$3:$D$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.7707083333333333</c:v>
@@ -2538,7 +2538,7 @@
             <c:numRef>
               <c:f>'cold start'!$L$3:$L$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.05945</c:v>
@@ -2607,7 +2607,7 @@
             <c:numRef>
               <c:f>'cold start'!$F$3:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>12.584279</c:v>
@@ -2757,28 +2757,28 @@
             <c:numRef>
               <c:f>'cold start'!$B$3:$B$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.311719999999999</c:v>
+                  <c:v>13.902771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0824500000000015</c:v>
+                  <c:v>9.5745090000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6768400000000003</c:v>
+                  <c:v>7.2162170000000012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.30016</c:v>
+                  <c:v>5.8561884999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4290000000000003</c:v>
+                  <c:v>4.8976600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7201111111111111</c:v>
+                  <c:v>4.1654125000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2016999999999998</c:v>
+                  <c:v>3.7020360000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2867,7 +2867,7 @@
             <c:numRef>
               <c:f>'cold start'!$J$3:$J$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>15.284255999999997</c:v>
@@ -3336,7 +3336,7 @@
             <c:numRef>
               <c:f>'cold start'!$D$3:$D$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.7707083333333333</c:v>
@@ -3391,7 +3391,7 @@
             <c:numRef>
               <c:f>'cold start'!$H$3:$H$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.7635500000000004</c:v>
@@ -3446,7 +3446,7 @@
             <c:numRef>
               <c:f>'cold start'!$L$3:$L$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.05945</c:v>
@@ -3784,7 +3784,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4033,28 +4033,28 @@
             <c:numRef>
               <c:f>'cold start'!$B$3:$B$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.311719999999999</c:v>
+                  <c:v>13.902771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0824500000000015</c:v>
+                  <c:v>9.5745090000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6768400000000003</c:v>
+                  <c:v>7.2162170000000012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.30016</c:v>
+                  <c:v>5.8561884999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4290000000000003</c:v>
+                  <c:v>4.8976600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7201111111111111</c:v>
+                  <c:v>4.1654125000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2016999999999998</c:v>
+                  <c:v>3.7020360000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4088,7 +4088,7 @@
             <c:numRef>
               <c:f>'cold start'!$F$3:$F$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>12.584279</c:v>
@@ -4143,7 +4143,7 @@
             <c:numRef>
               <c:f>'cold start'!$J$3:$J$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>15.284255999999997</c:v>
@@ -4482,7 +4482,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -13346,24 +13346,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -13727,11 +13727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22115D20-AEC8-E342-9EA8-01B34B7AB9E3}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13741,53 +13741,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57" t="s">
+      <c r="G1" s="60"/>
+      <c r="H1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="57"/>
-      <c r="J1" s="53" t="s">
+      <c r="I1" s="61"/>
+      <c r="J1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="48" t="s">
+      <c r="K1" s="57"/>
+      <c r="L1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="48"/>
+      <c r="M1" s="52"/>
       <c r="N1" s="37"/>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="50" t="s">
+      <c r="P1" s="53"/>
+      <c r="Q1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="51" t="s">
+      <c r="R1" s="54"/>
+      <c r="S1" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="52" t="s">
+      <c r="T1" s="55"/>
+      <c r="U1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="52"/>
+      <c r="V1" s="56"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -13856,68 +13856,68 @@
       <c r="A3" s="7">
         <v>128</v>
       </c>
-      <c r="B3" s="21">
-        <v>13.311719999999999</v>
-      </c>
-      <c r="C3" s="21">
-        <v>13.792399999999999</v>
-      </c>
-      <c r="D3" s="21">
+      <c r="B3" s="42">
+        <v>13.902771</v>
+      </c>
+      <c r="C3" s="42">
+        <v>14.136735999999999</v>
+      </c>
+      <c r="D3" s="42">
         <v>2.7707083333333333</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="42">
         <v>2.9409999999999998</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="42">
         <v>12.584279</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="42">
         <v>12.8475445</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="42">
         <v>2.7635500000000004</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="42">
         <v>3.7194500000000001</v>
       </c>
-      <c r="J3" s="21">
+      <c r="J3" s="42">
         <v>15.284255999999997</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="42">
         <v>15.6767825</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3" s="42">
         <v>3.05945</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="42">
         <v>3.1539999999999999</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="41">
         <f>1-L3/J3</f>
         <v>0.79982996882543711</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="42">
         <v>13.131603500000001</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="42">
         <v>13.437488999999999</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="42">
         <v>2.8224499999999999</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="42">
         <v>2.992</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="42">
         <v>14.531919</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="42">
         <v>14.970844999999999</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="42">
         <v>2.8411999999999997</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="42">
         <v>2.9591500000000002</v>
       </c>
     </row>
@@ -13925,68 +13925,68 @@
       <c r="A4" s="7">
         <v>192</v>
       </c>
-      <c r="B4" s="21">
-        <v>9.0824500000000015</v>
-      </c>
-      <c r="C4" s="21">
-        <v>9.1213300000000004</v>
-      </c>
-      <c r="D4" s="21">
+      <c r="B4" s="42">
+        <v>9.5745090000000008</v>
+      </c>
+      <c r="C4" s="42">
+        <v>9.9106820000000013</v>
+      </c>
+      <c r="D4" s="42">
         <v>2.2185999999999999</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="42">
         <v>2.3544</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="42">
         <v>8.6800315000000001</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="42">
         <v>9.0720564999999986</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="42">
         <v>2.1535500000000001</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="42">
         <v>2.3201499999999999</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="42">
         <v>10.867018499999997</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="42">
         <v>11.292242500000008</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="42">
         <v>2.55335</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="42">
         <v>2.6930500000000022</v>
       </c>
-      <c r="N4" s="27">
+      <c r="N4" s="41">
         <f t="shared" ref="N4:N9" si="0">1-L4/J4</f>
         <v>0.76503674858011872</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="42">
         <v>8.9549250000000011</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="42">
         <v>9.1351940000000003</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="42">
         <v>2.2601999999999998</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="42">
         <v>2.3608000000000002</v>
       </c>
-      <c r="S4" s="29">
+      <c r="S4" s="43">
         <v>9.9824789999999997</v>
       </c>
-      <c r="T4" s="29">
+      <c r="T4" s="43">
         <v>10.301406</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="42">
         <v>2.2308000000000003</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="42">
         <v>2.3284000000000002</v>
       </c>
     </row>
@@ -13994,68 +13994,68 @@
       <c r="A5" s="7">
         <v>256</v>
       </c>
-      <c r="B5" s="21">
-        <v>6.6768400000000003</v>
-      </c>
-      <c r="C5" s="21">
-        <v>6.8608000000000002</v>
-      </c>
-      <c r="D5" s="21">
+      <c r="B5" s="42">
+        <v>7.2162170000000012</v>
+      </c>
+      <c r="C5" s="42">
+        <v>7.4673034999999999</v>
+      </c>
+      <c r="D5" s="42">
         <v>1.9008333333333332</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="42">
         <v>2.1312500000000001</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="42">
         <v>6.2979319999999994</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="42">
         <v>6.4558615000000001</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="42">
         <v>1.8953</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="42">
         <v>2.0604500000000003</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="42">
         <v>7.7882359999999995</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="42">
         <v>8.0273275000000019</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="42">
         <v>2.0696500000000002</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="42">
         <v>2.2613000000000003</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="41">
         <f t="shared" si="0"/>
         <v>0.73425946517285812</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="42">
         <v>6.8351664999999997</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="42">
         <v>6.9901595000000007</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="42">
         <v>1.8931</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="42">
         <v>1.94425</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="42">
         <v>7.627080499999999</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="42">
         <v>7.9521390000000007</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="42">
         <v>1.8946000000000001</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="42">
         <v>1.9694</v>
       </c>
     </row>
@@ -14063,68 +14063,68 @@
       <c r="A6" s="7">
         <v>320</v>
       </c>
-      <c r="B6" s="21">
-        <v>5.30016</v>
-      </c>
-      <c r="C6" s="21">
-        <v>5.5291000000000006</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="B6" s="42">
+        <v>5.8561884999999991</v>
+      </c>
+      <c r="C6" s="42">
+        <v>6.0505819999999995</v>
+      </c>
+      <c r="D6" s="42">
         <v>1.6772799999999999</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="42">
         <v>1.7584000000000002</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="42">
         <v>5.3486039999999999</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="42">
         <v>5.5564615000000002</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="42">
         <v>1.7514000000000001</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="42">
         <v>2.2029999999999998</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="42">
         <v>6.4936315000000011</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="42">
         <v>7.1455015000000017</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="42">
         <v>1.9704000000000002</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="42">
         <v>2.2710000000000021</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="41">
         <f t="shared" si="0"/>
         <v>0.69656424144178808</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="42">
         <v>5.5005895000000002</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="42">
         <v>5.7364354999999998</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="42">
         <v>1.7212499999999999</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="42">
         <v>1.82955</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="42">
         <v>6.0706370000000005</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="42">
         <v>6.2845350000000009</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="42">
         <v>1.6910499999999999</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="42">
         <v>1.7534000000000001</v>
       </c>
     </row>
@@ -14132,68 +14132,68 @@
       <c r="A7" s="7">
         <v>384</v>
       </c>
-      <c r="B7" s="21">
-        <v>4.4290000000000003</v>
-      </c>
-      <c r="C7" s="21">
-        <v>4.5209999999999999</v>
-      </c>
-      <c r="D7" s="21">
+      <c r="B7" s="42">
+        <v>4.8976600000000001</v>
+      </c>
+      <c r="C7" s="42">
+        <v>5.069757000000001</v>
+      </c>
+      <c r="D7" s="42">
         <v>1.5789200000000001</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="42">
         <v>1.7197</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="42">
         <v>4.4421464999999998</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="42">
         <v>4.5426000000000002</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="42">
         <v>1.6086500000000001</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="42">
         <v>1.7222500000000001</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="42">
         <v>5.2042145000000009</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="42">
         <v>5.3488220000000002</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="42">
         <v>1.67875</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="42">
         <v>1.7477000000000003</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="41">
         <f t="shared" si="0"/>
         <v>0.67742490245165721</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="42">
         <v>4.5758350000000005</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="42">
         <v>4.7254869999999993</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="42">
         <v>1.6033499999999998</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="42">
         <v>1.6649500000000002</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="42">
         <v>5.0136354999999986</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="42">
         <v>5.1528295000000002</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="42">
         <v>1.5882499999999999</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="42">
         <v>1.6602000000000001</v>
       </c>
     </row>
@@ -14201,68 +14201,68 @@
       <c r="A8" s="7">
         <v>448</v>
       </c>
-      <c r="B8" s="21">
-        <v>3.7201111111111111</v>
-      </c>
-      <c r="C8" s="21">
-        <v>3.7754000000000003</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="B8" s="42">
+        <v>4.1654125000000004</v>
+      </c>
+      <c r="C8" s="42">
+        <v>4.2812825000000005</v>
+      </c>
+      <c r="D8" s="42">
         <v>1.4825599999999999</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="42">
         <v>1.5283</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="42">
         <v>3.8551370000000009</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="42">
         <v>3.9505850000000002</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="42">
         <v>1.56555</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="42">
         <v>1.7153</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="42">
         <v>4.5009115000000008</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="42">
         <v>4.7084974999999991</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="42">
         <v>1.5960000000000001</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="42">
         <v>1.7636500000000002</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="41">
         <f t="shared" si="0"/>
         <v>0.64540515848845281</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="42">
         <v>3.9798525000000007</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="42">
         <v>4.1028959999999994</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="42">
         <v>1.5258</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="42">
         <v>1.5828</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="42">
         <v>4.3454945</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="42">
         <v>4.4759270000000004</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="42">
         <v>1.5144500000000001</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="42">
         <v>1.5534000000000001</v>
       </c>
     </row>
@@ -14270,68 +14270,68 @@
       <c r="A9" s="7">
         <v>512</v>
       </c>
-      <c r="B9" s="21">
-        <v>3.2016999999999998</v>
-      </c>
-      <c r="C9" s="21">
-        <v>3.2849499999999998</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="B9" s="42">
+        <v>3.7020360000000001</v>
+      </c>
+      <c r="C9" s="42">
+        <v>3.8307094999999998</v>
+      </c>
+      <c r="D9" s="42">
         <v>1.4725652173913042</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="42">
         <v>1.6849999999999998</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="42">
         <v>3.4013584999999997</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="42">
         <v>3.5665500000000003</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="42">
         <v>1.5003499999999999</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="42">
         <v>1.6402000000000001</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="42">
         <v>3.9799080000000009</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="42">
         <v>4.0680405000000004</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="42">
         <v>1.5340597014925372</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="42">
         <v>1.6802999999999997</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="41">
         <f t="shared" si="0"/>
         <v>0.61454895402292298</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="42">
         <v>3.5054605000000003</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="42">
         <v>3.6048149999999999</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="42">
         <v>1.46055</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="42">
         <v>1.5424500000000001</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="42">
         <v>3.8091395000000001</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="42">
         <v>3.9268395000000003</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="42">
         <v>1.4807999999999999</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="42">
         <v>1.5562</v>
       </c>
     </row>
@@ -14456,6 +14456,7 @@
     <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -14476,75 +14477,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="50"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="30"/>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="63"/>
-      <c r="N1" s="64" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="64"/>
+      <c r="O1" s="68"/>
       <c r="P1" s="32"/>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="59"/>
-      <c r="S1" s="60" t="s">
+      <c r="R1" s="63"/>
+      <c r="S1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="60"/>
+      <c r="T1" s="64"/>
       <c r="U1" s="34"/>
-      <c r="V1" s="61" t="s">
+      <c r="V1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="62" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="62"/>
+      <c r="Y1" s="66"/>
       <c r="Z1" s="35"/>
-      <c r="AA1" s="56" t="s">
+      <c r="AA1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="57" t="s">
+      <c r="AB1" s="60"/>
+      <c r="AC1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="57"/>
+      <c r="AD1" s="61"/>
       <c r="AE1" s="36"/>
-      <c r="AF1" s="65" t="s">
+      <c r="AF1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="66" t="s">
+      <c r="AG1" s="69"/>
+      <c r="AH1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="66"/>
+      <c r="AI1" s="70"/>
       <c r="AJ1" s="38"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14667,7 +14668,7 @@
       <c r="E3" s="21">
         <v>519.1</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="41">
         <f>1-D3/B3</f>
         <v>5.5833934022036735E-2</v>
       </c>
@@ -14683,7 +14684,7 @@
       <c r="J3" s="21">
         <v>771.30000000000007</v>
       </c>
-      <c r="K3" s="67">
+      <c r="K3" s="41">
         <f>1-I3/G3</f>
         <v>6.2411719344502403E-2</v>
       </c>
@@ -14699,7 +14700,7 @@
       <c r="O3">
         <v>1145.5500000000002</v>
       </c>
-      <c r="P3" s="67">
+      <c r="P3" s="41">
         <f>1-N3/L3</f>
         <v>0.21016725493084965</v>
       </c>
@@ -14715,7 +14716,7 @@
       <c r="T3">
         <v>696.05000000000007</v>
       </c>
-      <c r="U3" s="67">
+      <c r="U3" s="41">
         <f>1-S3/Q3</f>
         <v>0.38039275930050953</v>
       </c>
@@ -14731,23 +14732,23 @@
       <c r="Y3">
         <v>5841.7</v>
       </c>
-      <c r="Z3" s="67">
+      <c r="Z3" s="41">
         <f>1-X3/V3</f>
         <v>0.14793472775325645</v>
       </c>
-      <c r="AA3" s="68">
+      <c r="AA3" s="42">
         <v>12584.279</v>
       </c>
-      <c r="AB3" s="68">
+      <c r="AB3" s="42">
         <v>12847.5445</v>
       </c>
-      <c r="AC3" s="68">
+      <c r="AC3" s="42">
         <v>2763.55</v>
       </c>
-      <c r="AD3" s="68">
+      <c r="AD3" s="42">
         <v>3719.4500000000003</v>
       </c>
-      <c r="AE3" s="67">
+      <c r="AE3" s="41">
         <f>1-AC3/AA3</f>
         <v>0.78039663615213872</v>
       </c>
@@ -14763,7 +14764,7 @@
       <c r="AI3">
         <v>726.55</v>
       </c>
-      <c r="AJ3" s="67">
+      <c r="AJ3" s="41">
         <f t="shared" ref="AJ3:AJ8" si="0">1-AH3/AF3</f>
         <v>-9.3174136328073365E-2</v>
       </c>
@@ -14784,7 +14785,7 @@
       <c r="E4" s="21">
         <v>398.1</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="41">
         <f t="shared" ref="F4:F9" si="1">1-D4/B4</f>
         <v>2.6579607416876594E-2</v>
       </c>
@@ -14800,7 +14801,7 @@
       <c r="J4" s="21">
         <v>649.15</v>
       </c>
-      <c r="K4" s="67">
+      <c r="K4" s="41">
         <f t="shared" ref="K4:K9" si="2">1-I4/G4</f>
         <v>6.1931890775252851E-2</v>
       </c>
@@ -14816,7 +14817,7 @@
       <c r="O4">
         <v>913.00000000000011</v>
       </c>
-      <c r="P4" s="67">
+      <c r="P4" s="41">
         <f t="shared" ref="P4:P9" si="3">1-N4/L4</f>
         <v>0.19360501055261359</v>
       </c>
@@ -14832,7 +14833,7 @@
       <c r="T4">
         <v>587.75</v>
       </c>
-      <c r="U4" s="67">
+      <c r="U4" s="41">
         <f t="shared" ref="U4:U9" si="4">1-S4/Q4</f>
         <v>0.35172752844815802</v>
       </c>
@@ -14848,23 +14849,23 @@
       <c r="Y4">
         <v>4203.9500000000007</v>
       </c>
-      <c r="Z4" s="67">
+      <c r="Z4" s="41">
         <f t="shared" ref="Z4:Z9" si="5">1-X4/V4</f>
         <v>0.13277589431743808</v>
       </c>
-      <c r="AA4" s="68">
+      <c r="AA4" s="42">
         <v>8680.031500000001</v>
       </c>
-      <c r="AB4" s="68">
+      <c r="AB4" s="42">
         <v>9072.0564999999988</v>
       </c>
-      <c r="AC4" s="68">
+      <c r="AC4" s="42">
         <v>2153.5500000000002</v>
       </c>
-      <c r="AD4" s="68">
+      <c r="AD4" s="42">
         <v>2320.15</v>
       </c>
-      <c r="AE4" s="67">
+      <c r="AE4" s="41">
         <f t="shared" ref="AE4:AE9" si="6">1-AC4/AA4</f>
         <v>0.7518960616675181</v>
       </c>
@@ -14880,7 +14881,7 @@
       <c r="AI4">
         <v>545.04999999999995</v>
       </c>
-      <c r="AJ4" s="67">
+      <c r="AJ4" s="41">
         <f t="shared" si="0"/>
         <v>-0.12696409891401639</v>
       </c>
@@ -14901,7 +14902,7 @@
       <c r="E5" s="21">
         <v>376.90000000000015</v>
       </c>
-      <c r="F5" s="67">
+      <c r="F5" s="41">
         <f t="shared" si="1"/>
         <v>-7.9280134913822131E-2</v>
       </c>
@@ -14917,7 +14918,7 @@
       <c r="J5" s="21">
         <v>588.15000000000009</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="41">
         <f t="shared" si="2"/>
         <v>6.8002842663328344E-2</v>
       </c>
@@ -14933,7 +14934,7 @@
       <c r="O5">
         <v>901.05000000000007</v>
       </c>
-      <c r="P5" s="67">
+      <c r="P5" s="41">
         <f t="shared" si="3"/>
         <v>0.18418994717230208</v>
       </c>
@@ -14949,7 +14950,7 @@
       <c r="T5">
         <v>549</v>
       </c>
-      <c r="U5" s="67">
+      <c r="U5" s="41">
         <f t="shared" si="4"/>
         <v>0.3234057044223313</v>
       </c>
@@ -14965,23 +14966,23 @@
       <c r="Y5">
         <v>3125</v>
       </c>
-      <c r="Z5" s="67">
+      <c r="Z5" s="41">
         <f t="shared" si="5"/>
         <v>0.14634669477451423</v>
       </c>
-      <c r="AA5" s="68">
+      <c r="AA5" s="42">
         <v>6297.9319999999998</v>
       </c>
-      <c r="AB5" s="68">
+      <c r="AB5" s="42">
         <v>6455.8615</v>
       </c>
-      <c r="AC5" s="68">
+      <c r="AC5" s="42">
         <v>1895.3</v>
       </c>
-      <c r="AD5" s="68">
+      <c r="AD5" s="42">
         <v>2060.4500000000003</v>
       </c>
-      <c r="AE5" s="67">
+      <c r="AE5" s="41">
         <f t="shared" si="6"/>
         <v>0.69905994539159844</v>
       </c>
@@ -14997,7 +14998,7 @@
       <c r="AI5" s="39">
         <v>432.3</v>
       </c>
-      <c r="AJ5" s="67">
+      <c r="AJ5" s="41">
         <f t="shared" si="0"/>
         <v>-0.16670224937456557</v>
       </c>
@@ -15018,7 +15019,7 @@
       <c r="E6" s="21">
         <v>310.35000000000002</v>
       </c>
-      <c r="F6" s="67">
+      <c r="F6" s="41">
         <f t="shared" si="1"/>
         <v>-3.8883380787015254E-2</v>
       </c>
@@ -15034,7 +15035,7 @@
       <c r="J6" s="21">
         <v>692.80000000000007</v>
       </c>
-      <c r="K6" s="67">
+      <c r="K6" s="41">
         <f t="shared" si="2"/>
         <v>1.7048549794708157E-2</v>
       </c>
@@ -15050,7 +15051,7 @@
       <c r="O6">
         <v>881.3</v>
       </c>
-      <c r="P6" s="67">
+      <c r="P6" s="41">
         <f t="shared" si="3"/>
         <v>0.18707655305307913</v>
       </c>
@@ -15066,7 +15067,7 @@
       <c r="T6">
         <v>521.29999999999995</v>
       </c>
-      <c r="U6" s="67">
+      <c r="U6" s="41">
         <f t="shared" si="4"/>
         <v>0.30116463299856</v>
       </c>
@@ -15082,23 +15083,23 @@
       <c r="Y6">
         <v>2613.4</v>
       </c>
-      <c r="Z6" s="67">
+      <c r="Z6" s="41">
         <f t="shared" si="5"/>
         <v>0.14880437199408048</v>
       </c>
-      <c r="AA6" s="68">
+      <c r="AA6" s="42">
         <v>5348.6040000000003</v>
       </c>
-      <c r="AB6" s="68">
+      <c r="AB6" s="42">
         <v>5556.4615000000003</v>
       </c>
-      <c r="AC6" s="68">
+      <c r="AC6" s="42">
         <v>1751.4</v>
       </c>
-      <c r="AD6" s="68">
+      <c r="AD6" s="42">
         <v>2203</v>
       </c>
-      <c r="AE6" s="67">
+      <c r="AE6" s="41">
         <f t="shared" si="6"/>
         <v>0.67255007100918296</v>
       </c>
@@ -15114,7 +15115,7 @@
       <c r="AI6" s="29">
         <v>393.05</v>
       </c>
-      <c r="AJ6" s="67">
+      <c r="AJ6" s="41">
         <f t="shared" si="0"/>
         <v>-0.1784779109338468</v>
       </c>
@@ -15135,7 +15136,7 @@
       <c r="E7" s="21">
         <v>314.25000000000006</v>
       </c>
-      <c r="F7" s="67">
+      <c r="F7" s="41">
         <f t="shared" si="1"/>
         <v>-0.13318749591514267</v>
       </c>
@@ -15151,7 +15152,7 @@
       <c r="J7" s="21">
         <v>668.45</v>
       </c>
-      <c r="K7" s="67">
+      <c r="K7" s="41">
         <f t="shared" si="2"/>
         <v>4.2218045435103102E-2</v>
       </c>
@@ -15167,7 +15168,7 @@
       <c r="O7">
         <v>903.80000000000007</v>
       </c>
-      <c r="P7" s="67">
+      <c r="P7" s="41">
         <f t="shared" si="3"/>
         <v>0.17635508311291204</v>
       </c>
@@ -15183,7 +15184,7 @@
       <c r="T7">
         <v>512.25</v>
       </c>
-      <c r="U7" s="67">
+      <c r="U7" s="41">
         <f t="shared" si="4"/>
         <v>0.2768007822509152</v>
       </c>
@@ -15199,23 +15200,23 @@
       <c r="Y7">
         <v>2260.6</v>
       </c>
-      <c r="Z7" s="67">
+      <c r="Z7" s="41">
         <f t="shared" si="5"/>
         <v>0.15546448573519356</v>
       </c>
-      <c r="AA7" s="68">
+      <c r="AA7" s="42">
         <v>4442.1464999999998</v>
       </c>
-      <c r="AB7" s="68">
+      <c r="AB7" s="42">
         <v>4542.6000000000004</v>
       </c>
-      <c r="AC7" s="68">
+      <c r="AC7" s="42">
         <v>1608.65</v>
       </c>
-      <c r="AD7" s="68">
+      <c r="AD7" s="42">
         <v>1722.25</v>
       </c>
-      <c r="AE7" s="67">
+      <c r="AE7" s="41">
         <f t="shared" si="6"/>
         <v>0.63786651340742584</v>
       </c>
@@ -15231,7 +15232,7 @@
       <c r="AI7" s="29">
         <v>374.50000000000017</v>
       </c>
-      <c r="AJ7" s="67">
+      <c r="AJ7" s="41">
         <f t="shared" si="0"/>
         <v>-0.21739903141244921</v>
       </c>
@@ -15252,7 +15253,7 @@
       <c r="E8" s="21">
         <v>310.30000000000013</v>
       </c>
-      <c r="F8" s="67">
+      <c r="F8" s="41">
         <f t="shared" si="1"/>
         <v>-0.14232110718782964</v>
       </c>
@@ -15268,7 +15269,7 @@
       <c r="J8" s="21">
         <v>657.8</v>
       </c>
-      <c r="K8" s="67">
+      <c r="K8" s="41">
         <f t="shared" si="2"/>
         <v>3.0868132930943148E-2</v>
       </c>
@@ -15284,7 +15285,7 @@
       <c r="O8">
         <v>908.10000000000014</v>
       </c>
-      <c r="P8" s="67">
+      <c r="P8" s="41">
         <f t="shared" si="3"/>
         <v>0.17465441862189512</v>
       </c>
@@ -15300,7 +15301,7 @@
       <c r="T8">
         <v>501.1</v>
       </c>
-      <c r="U8" s="67">
+      <c r="U8" s="41">
         <f t="shared" si="4"/>
         <v>0.2520008800907555</v>
       </c>
@@ -15316,23 +15317,23 @@
       <c r="Y8">
         <v>2013.9</v>
       </c>
-      <c r="Z8" s="67">
+      <c r="Z8" s="41">
         <f t="shared" si="5"/>
         <v>0.15739746637150331</v>
       </c>
-      <c r="AA8" s="68">
+      <c r="AA8" s="42">
         <v>3855.1370000000011</v>
       </c>
-      <c r="AB8" s="68">
+      <c r="AB8" s="42">
         <v>3950.585</v>
       </c>
-      <c r="AC8" s="68">
+      <c r="AC8" s="42">
         <v>1565.55</v>
       </c>
-      <c r="AD8" s="68">
+      <c r="AD8" s="42">
         <v>1715.3</v>
       </c>
-      <c r="AE8" s="67">
+      <c r="AE8" s="41">
         <f t="shared" si="6"/>
         <v>0.59390548247701713</v>
       </c>
@@ -15348,7 +15349,7 @@
       <c r="AI8">
         <v>329.25000000000006</v>
       </c>
-      <c r="AJ8" s="67">
+      <c r="AJ8" s="41">
         <f t="shared" si="0"/>
         <v>-0.2570320537249895</v>
       </c>
@@ -15369,7 +15370,7 @@
       <c r="E9" s="21">
         <v>277.3</v>
       </c>
-      <c r="F9" s="67">
+      <c r="F9" s="41">
         <f t="shared" si="1"/>
         <v>-0.1277446801298292</v>
       </c>
@@ -15385,7 +15386,7 @@
       <c r="J9" s="21">
         <v>571.85</v>
       </c>
-      <c r="K9" s="67">
+      <c r="K9" s="41">
         <f t="shared" si="2"/>
         <v>4.3051411386417437E-2</v>
       </c>
@@ -15401,7 +15402,7 @@
       <c r="O9">
         <v>883.9</v>
       </c>
-      <c r="P9" s="67">
+      <c r="P9" s="41">
         <f t="shared" si="3"/>
         <v>0.18331991640071821</v>
       </c>
@@ -15417,7 +15418,7 @@
       <c r="T9">
         <v>489.15</v>
       </c>
-      <c r="U9" s="67">
+      <c r="U9" s="41">
         <f t="shared" si="4"/>
         <v>0.24972109110278617</v>
       </c>
@@ -15433,23 +15434,23 @@
       <c r="Y9">
         <v>1848.95</v>
       </c>
-      <c r="Z9" s="67">
+      <c r="Z9" s="41">
         <f t="shared" si="5"/>
         <v>0.13742937220313645</v>
       </c>
-      <c r="AA9" s="68">
+      <c r="AA9" s="42">
         <v>3401.3584999999998</v>
       </c>
-      <c r="AB9" s="68">
+      <c r="AB9" s="42">
         <v>3566.55</v>
       </c>
-      <c r="AC9" s="68">
+      <c r="AC9" s="42">
         <v>1500.35</v>
       </c>
-      <c r="AD9" s="68">
+      <c r="AD9" s="42">
         <v>1640.2</v>
       </c>
-      <c r="AE9" s="67">
+      <c r="AE9" s="41">
         <f t="shared" si="6"/>
         <v>0.55889683489699782</v>
       </c>
@@ -15465,7 +15466,7 @@
       <c r="AI9">
         <v>310.65000000000003</v>
       </c>
-      <c r="AJ9" s="67">
+      <c r="AJ9" s="41">
         <f>1-AH9/AF9</f>
         <v>-0.27706569106523049</v>
       </c>
@@ -15474,16 +15475,16 @@
       <c r="A10" s="7">
         <v>576</v>
       </c>
-      <c r="AA10" s="68">
+      <c r="AA10" s="42">
         <v>2967.4119999999994</v>
       </c>
-      <c r="AB10" s="68">
+      <c r="AB10" s="42">
         <v>3068.2339999999999</v>
       </c>
-      <c r="AC10" s="68">
+      <c r="AC10" s="42">
         <v>1418.15</v>
       </c>
-      <c r="AD10" s="68">
+      <c r="AD10" s="42">
         <v>1532.65</v>
       </c>
     </row>
@@ -15491,16 +15492,16 @@
       <c r="A11" s="7">
         <v>640</v>
       </c>
-      <c r="AA11" s="68">
+      <c r="AA11" s="42">
         <v>2704.2674999999995</v>
       </c>
-      <c r="AB11" s="68">
+      <c r="AB11" s="42">
         <v>2794.0855000000001</v>
       </c>
-      <c r="AC11" s="68">
+      <c r="AC11" s="42">
         <v>1345.65</v>
       </c>
-      <c r="AD11" s="68">
+      <c r="AD11" s="42">
         <v>1423.65</v>
       </c>
     </row>
@@ -15508,16 +15509,16 @@
       <c r="A12" s="7">
         <v>704</v>
       </c>
-      <c r="AA12" s="68">
+      <c r="AA12" s="42">
         <v>2488.4484999999995</v>
       </c>
-      <c r="AB12" s="68">
+      <c r="AB12" s="42">
         <v>2597.2195000000002</v>
       </c>
-      <c r="AC12" s="68">
+      <c r="AC12" s="42">
         <v>1453</v>
       </c>
-      <c r="AD12" s="68">
+      <c r="AD12" s="42">
         <v>1539.7500000000016</v>
       </c>
     </row>
@@ -15525,16 +15526,16 @@
       <c r="A13" s="7">
         <v>768</v>
       </c>
-      <c r="AA13" s="68">
+      <c r="AA13" s="42">
         <v>2297.357</v>
       </c>
-      <c r="AB13" s="68">
+      <c r="AB13" s="42">
         <v>2346.4409999999998</v>
       </c>
-      <c r="AC13" s="68">
+      <c r="AC13" s="42">
         <v>1332.8</v>
       </c>
-      <c r="AD13" s="68">
+      <c r="AD13" s="42">
         <v>1407.0500000000002</v>
       </c>
     </row>
@@ -15542,16 +15543,16 @@
       <c r="A14" s="7">
         <v>832</v>
       </c>
-      <c r="AA14" s="68">
+      <c r="AA14" s="42">
         <v>2175.2925</v>
       </c>
-      <c r="AB14" s="68">
+      <c r="AB14" s="42">
         <v>2235.64</v>
       </c>
-      <c r="AC14" s="68">
+      <c r="AC14" s="42">
         <v>1332.45</v>
       </c>
-      <c r="AD14" s="68">
+      <c r="AD14" s="42">
         <v>1396.1000000000001</v>
       </c>
     </row>
@@ -15559,16 +15560,16 @@
       <c r="A15" s="7">
         <v>896</v>
       </c>
-      <c r="AA15" s="68">
+      <c r="AA15" s="42">
         <v>2038.9569999999999</v>
       </c>
-      <c r="AB15" s="68">
+      <c r="AB15" s="42">
         <v>2099.6795000000002</v>
       </c>
-      <c r="AC15" s="68">
+      <c r="AC15" s="42">
         <v>1295.25</v>
       </c>
-      <c r="AD15" s="68">
+      <c r="AD15" s="42">
         <v>1339.3500000000001</v>
       </c>
     </row>
@@ -15576,22 +15577,22 @@
       <c r="A16" s="7">
         <v>960</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
       <c r="F16" s="33"/>
       <c r="Q16">
         <v>1</v>
       </c>
-      <c r="AA16" s="69">
+      <c r="AA16" s="43">
         <v>1944.2395000000001</v>
       </c>
-      <c r="AB16" s="69">
+      <c r="AB16" s="43">
         <v>1997.9580000000001</v>
       </c>
-      <c r="AC16" s="68">
+      <c r="AC16" s="42">
         <v>1329.0526315789473</v>
       </c>
-      <c r="AD16" s="68">
+      <c r="AD16" s="42">
         <v>1609.3</v>
       </c>
     </row>
@@ -15602,16 +15603,16 @@
       <c r="Q17">
         <v>14</v>
       </c>
-      <c r="AA17" s="69">
+      <c r="AA17" s="43">
         <v>1852.7779999999996</v>
       </c>
-      <c r="AB17" s="69">
+      <c r="AB17" s="43">
         <v>1926.6369999999999</v>
       </c>
-      <c r="AC17" s="68">
+      <c r="AC17" s="42">
         <v>1275.4000000000001</v>
       </c>
-      <c r="AD17" s="68">
+      <c r="AD17" s="42">
         <v>1340.7500000000002</v>
       </c>
     </row>
@@ -15626,16 +15627,16 @@
       <c r="Q18">
         <v>64</v>
       </c>
-      <c r="AA18" s="68">
+      <c r="AA18" s="42">
         <v>1250.7869999999998</v>
       </c>
-      <c r="AB18" s="68">
+      <c r="AB18" s="42">
         <v>1288.0135</v>
       </c>
-      <c r="AC18" s="68">
+      <c r="AC18" s="42">
         <v>1245.5999999999999</v>
       </c>
-      <c r="AD18" s="68">
+      <c r="AD18" s="42">
         <v>1429.6000000000001</v>
       </c>
     </row>
@@ -15650,16 +15651,16 @@
       <c r="Q19">
         <v>83</v>
       </c>
-      <c r="AA19" s="68">
+      <c r="AA19" s="42">
         <v>1205.6444999999999</v>
       </c>
-      <c r="AB19" s="68">
+      <c r="AB19" s="42">
         <v>1236.9480000000001</v>
       </c>
-      <c r="AC19" s="70">
+      <c r="AC19" s="44">
         <v>1194.7142857142858</v>
       </c>
-      <c r="AD19" s="70">
+      <c r="AD19" s="44">
         <v>1251.3999999999999</v>
       </c>
     </row>
@@ -15792,7 +15793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C7387A-1CBC-9545-9516-2C253950AE23}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="172" workbookViewId="0">
+    <sheetView topLeftCell="F18" zoomScale="172" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -15803,20 +15804,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added tests and new apps for the java applications
</commit_message>
<xml_diff>
--- a/experiments/lambda/analysis_run_cold.xlsx
+++ b/experiments/lambda/analysis_run_cold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimedantas/Documents/git/serverless-iot-deployment/experiments/lambda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA462CE-DDA3-F84D-8C63-D59C7AACEC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6692571A-1351-C140-A78F-7A791029CB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
   <si>
     <t>Memory</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>factorial zip</t>
+  </si>
+  <si>
+    <t>per</t>
   </si>
 </sst>
 </file>
@@ -14494,9 +14497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DE693F-DFBF-A645-98AD-B3E2E7E6F16B}">
   <dimension ref="A1:AJ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="113" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A18:A24"/>
+      <selection pane="topRight" activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15625,7 +15628,7 @@
         <v>1609.3</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>1024</v>
       </c>
@@ -15649,7 +15652,7 @@
         <v>0.31162826847037239</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>1088</v>
       </c>
@@ -15668,8 +15671,12 @@
       <c r="AD18" s="42">
         <v>1568.2999999999995</v>
       </c>
+      <c r="AE18" s="73">
+        <f t="shared" ref="AE18:AE24" si="7">1-AC18/AA18</f>
+        <v>0.24684477040523256</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>1152</v>
       </c>
@@ -15688,8 +15695,12 @@
       <c r="AD19" s="42">
         <v>1409.8500000000001</v>
       </c>
+      <c r="AE19" s="73">
+        <f t="shared" si="7"/>
+        <v>0.24315813720468904</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>1216</v>
       </c>
@@ -15708,8 +15719,12 @@
       <c r="AD20" s="42">
         <v>1406</v>
       </c>
+      <c r="AE20" s="73">
+        <f t="shared" si="7"/>
+        <v>0.2107580828730059</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>1280</v>
       </c>
@@ -15728,8 +15743,12 @@
       <c r="AD21" s="42">
         <v>1361.3500000000001</v>
       </c>
+      <c r="AE21" s="73">
+        <f t="shared" si="7"/>
+        <v>0.18685773770110026</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>1344</v>
       </c>
@@ -15748,8 +15767,12 @@
       <c r="AD22" s="42">
         <v>1479.65</v>
       </c>
+      <c r="AE22" s="73">
+        <f t="shared" si="7"/>
+        <v>0.14910522848791985</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>1408</v>
       </c>
@@ -15768,8 +15791,15 @@
       <c r="AD23" s="42">
         <v>1381.3000000000002</v>
       </c>
+      <c r="AE23" s="73">
+        <f t="shared" si="7"/>
+        <v>0.12952252491603822</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>1472</v>
       </c>
@@ -15788,8 +15818,16 @@
       <c r="AD24">
         <v>1574.75</v>
       </c>
+      <c r="AE24" s="73">
+        <f>1-AC24/AA24</f>
+        <v>8.0012704851804672E-2</v>
+      </c>
+      <c r="AF24" s="72">
+        <f>1-AD24/AB24</f>
+        <v>-5.1915424597085646E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>2048</v>
       </c>
@@ -15817,7 +15855,7 @@
         <v>4.1469890556904421E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>3008</v>
       </c>
@@ -15845,26 +15883,26 @@
         <v>9.0658683266203743E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="G27" s="27"/>
       <c r="Q27">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="G28" s="27"/>
       <c r="Q28">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="G29" s="27"/>
       <c r="Q29">
         <v>230</v>
       </c>
       <c r="AC29" s="28"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>

</xml_diff>

<commit_message>
Added matlab tests and node apps
</commit_message>
<xml_diff>
--- a/experiments/lambda/analysis_run_cold.xlsx
+++ b/experiments/lambda/analysis_run_cold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimedantas/Documents/git/serverless-iot-deployment/experiments/lambda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6692571A-1351-C140-A78F-7A791029CB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E34C7-2EE3-0741-8C87-1DC4546B0C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{1003A129-F681-6E44-B98C-F95A01010A8D}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="31">
   <si>
     <t>Memory</t>
   </si>
@@ -120,6 +120,24 @@
   <si>
     <t>per</t>
   </si>
+  <si>
+    <t>node 234mb zip</t>
+  </si>
+  <si>
+    <t>node 78mb zip</t>
+  </si>
+  <si>
+    <t>Java 133mb zip</t>
+  </si>
+  <si>
+    <t>Java 15mb zip</t>
+  </si>
+  <si>
+    <t>Java factorial 10mb zip</t>
+  </si>
+  <si>
+    <t>node factorial 6byte zip</t>
+  </si>
 </sst>
 </file>
 
@@ -129,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,8 +174,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +246,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -381,6 +430,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,21 +462,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -432,10 +476,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -459,8 +512,36 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13355,24 +13436,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="46"/>
+      <c r="A2" s="56"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -13751,53 +13832,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57" t="s">
+      <c r="G1" s="71"/>
+      <c r="H1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="57"/>
-      <c r="J1" s="53" t="s">
+      <c r="I1" s="72"/>
+      <c r="J1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="58" t="s">
+      <c r="K1" s="68"/>
+      <c r="L1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="58"/>
+      <c r="M1" s="63"/>
       <c r="N1" s="37"/>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="60" t="s">
+      <c r="P1" s="64"/>
+      <c r="Q1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="60"/>
-      <c r="S1" s="61" t="s">
+      <c r="R1" s="65"/>
+      <c r="S1" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="61"/>
-      <c r="U1" s="62" t="s">
+      <c r="T1" s="66"/>
+      <c r="U1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="62"/>
+      <c r="V1" s="67"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="69"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14376,20 +14457,20 @@
       <c r="I14" s="21"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C16" s="72">
+      <c r="C16" s="46">
         <f>(B5-S5)/S5</f>
         <v>-5.3869039405051236E-2</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="46">
         <f>(D5-U5)/D5</f>
         <v>3.2792634809292896E-3</v>
       </c>
     </row>
     <row r="17" spans="7:20" x14ac:dyDescent="0.2">
-      <c r="G17" s="73">
+      <c r="G17" s="47">
         <v>5.3869039405051201E-2</v>
       </c>
-      <c r="H17" s="73">
+      <c r="H17" s="47">
         <v>3.2792634809292896E-3</v>
       </c>
       <c r="I17" s="2">
@@ -14475,17 +14556,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -14495,11 +14576,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DE693F-DFBF-A645-98AD-B3E2E7E6F16B}">
-  <dimension ref="A1:AJ55"/>
+  <dimension ref="A1:BN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="113" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="113" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BJ3" sqref="BJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14508,76 +14589,130 @@
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="70"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="60"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="30"/>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="71" t="s">
+      <c r="M1" s="78"/>
+      <c r="N1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="71"/>
+      <c r="O1" s="79"/>
       <c r="P1" s="32"/>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="66"/>
-      <c r="S1" s="67" t="s">
+      <c r="R1" s="74"/>
+      <c r="S1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="67"/>
+      <c r="T1" s="75"/>
       <c r="U1" s="34"/>
-      <c r="V1" s="68" t="s">
+      <c r="V1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="69" t="s">
+      <c r="W1" s="76"/>
+      <c r="X1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="69"/>
+      <c r="Y1" s="77"/>
       <c r="Z1" s="35"/>
-      <c r="AA1" s="56" t="s">
+      <c r="AA1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="57" t="s">
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="57"/>
+      <c r="AD1" s="72"/>
       <c r="AE1" s="36"/>
-      <c r="AF1" s="63" t="s">
+      <c r="AF1" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="64" t="s">
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="64"/>
+      <c r="AI1" s="81"/>
       <c r="AJ1" s="38"/>
+      <c r="AK1" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN1" s="83"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS1" s="85"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV1" s="86"/>
+      <c r="AW1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX1" s="87"/>
+      <c r="AY1" s="55"/>
+      <c r="AZ1" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA1" s="76"/>
+      <c r="BB1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="51"/>
+      <c r="BE1" s="88" t="s">
+        <v>28</v>
+      </c>
+      <c r="BF1" s="88"/>
+      <c r="BG1" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH1" s="89"/>
+      <c r="BI1" s="53"/>
+      <c r="BJ1" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="BK1" s="66"/>
+      <c r="BL1" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="54"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A2" s="69"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -14683,8 +14818,98 @@
       <c r="AJ2" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="AK2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>128</v>
       </c>
@@ -14800,8 +15025,104 @@
         <f t="shared" ref="AJ3:AJ8" si="0">1-AH3/AF3</f>
         <v>-9.3174136328073365E-2</v>
       </c>
+      <c r="AK3">
+        <v>2731.6055000000006</v>
+      </c>
+      <c r="AL3">
+        <v>3295.2285000000002</v>
+      </c>
+      <c r="AM3">
+        <v>2569.15</v>
+      </c>
+      <c r="AN3">
+        <v>3682.85</v>
+      </c>
+      <c r="AO3" s="41">
+        <f>1-AM3/AK3</f>
+        <v>5.9472533643675995E-2</v>
+      </c>
+      <c r="AP3">
+        <v>1604.1535000000001</v>
+      </c>
+      <c r="AQ3">
+        <v>1712.912</v>
+      </c>
+      <c r="AR3">
+        <v>1514.25</v>
+      </c>
+      <c r="AS3">
+        <v>1610.65</v>
+      </c>
+      <c r="AT3" s="41">
+        <f>1-AR3/AP3</f>
+        <v>5.6044200258890453E-2</v>
+      </c>
+      <c r="AU3">
+        <v>180.733</v>
+      </c>
+      <c r="AV3">
+        <v>199.26400000000001</v>
+      </c>
+      <c r="AW3">
+        <v>257</v>
+      </c>
+      <c r="AX3">
+        <v>334.55</v>
+      </c>
+      <c r="AY3" s="41">
+        <f>1-AW3/AU3</f>
+        <v>-0.42198713018651812</v>
+      </c>
+      <c r="AZ3">
+        <v>14503.405499999999</v>
+      </c>
+      <c r="BA3">
+        <v>15548.220000000001</v>
+      </c>
+      <c r="BB3">
+        <v>20892.95</v>
+      </c>
+      <c r="BC3">
+        <v>22870.850000000002</v>
+      </c>
+      <c r="BD3" s="41">
+        <f>1-BB3/AZ3</f>
+        <v>-0.44055477177411895</v>
+      </c>
+      <c r="BE3">
+        <v>1820.6125</v>
+      </c>
+      <c r="BF3">
+        <v>1879.135</v>
+      </c>
+      <c r="BG3">
+        <v>1792.15</v>
+      </c>
+      <c r="BH3">
+        <v>1902.6</v>
+      </c>
+      <c r="BI3" s="41">
+        <f>1-BG3/BE3</f>
+        <v>1.5633474998111851E-2</v>
+      </c>
+      <c r="BJ3">
+        <v>793.9235000000001</v>
+      </c>
+      <c r="BK3">
+        <v>931.05050000000006</v>
+      </c>
+      <c r="BL3">
+        <v>855.2</v>
+      </c>
+      <c r="BM3">
+        <v>967.85</v>
+      </c>
+      <c r="BN3" s="41">
+        <f>1-BL3/BJ3</f>
+        <v>-7.7181869537807923E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>192</v>
       </c>
@@ -14917,8 +15238,104 @@
         <f t="shared" si="0"/>
         <v>-0.12696409891401639</v>
       </c>
+      <c r="AK4">
+        <v>2043.7220000000002</v>
+      </c>
+      <c r="AL4">
+        <v>2122.7725</v>
+      </c>
+      <c r="AM4">
+        <v>2177.8000000000002</v>
+      </c>
+      <c r="AN4">
+        <v>2491.9500000000003</v>
+      </c>
+      <c r="AO4" s="41">
+        <f t="shared" ref="AO4:AO9" si="7">1-AM4/AK4</f>
+        <v>-6.5604813179091837E-2</v>
+      </c>
+      <c r="AP4" s="49">
+        <v>1894.4955000000002</v>
+      </c>
+      <c r="AQ4" s="49">
+        <v>2150.971</v>
+      </c>
+      <c r="AR4">
+        <v>1874.45</v>
+      </c>
+      <c r="AS4">
+        <v>2136.8000000000002</v>
+      </c>
+      <c r="AT4" s="41">
+        <f t="shared" ref="AT4:AT9" si="8">1-AR4/AP4</f>
+        <v>1.058091718877141E-2</v>
+      </c>
+      <c r="AU4">
+        <v>176.46899999999997</v>
+      </c>
+      <c r="AV4">
+        <v>195.00749999999999</v>
+      </c>
+      <c r="AW4">
+        <v>258.25</v>
+      </c>
+      <c r="AX4">
+        <v>303.95000000000005</v>
+      </c>
+      <c r="AY4" s="41">
+        <f>1-AW4/AU4</f>
+        <v>-0.46342983753520484</v>
+      </c>
+      <c r="AZ4">
+        <v>9721.8280000000013</v>
+      </c>
+      <c r="BA4">
+        <v>10077.89</v>
+      </c>
+      <c r="BB4">
+        <v>14135.55</v>
+      </c>
+      <c r="BC4">
+        <v>15348.25</v>
+      </c>
+      <c r="BD4" s="41">
+        <f t="shared" ref="BD4:BD9" si="9">1-BB4/AZ4</f>
+        <v>-0.4540012433875602</v>
+      </c>
+      <c r="BE4">
+        <v>1340.4235000000003</v>
+      </c>
+      <c r="BF4">
+        <v>1423.7159999999999</v>
+      </c>
+      <c r="BG4">
+        <v>1382.3</v>
+      </c>
+      <c r="BH4">
+        <v>1462.05</v>
+      </c>
+      <c r="BI4" s="41">
+        <f t="shared" ref="BI4:BI9" si="10">1-BG4/BE4</f>
+        <v>-3.1241245770459614E-2</v>
+      </c>
+      <c r="BJ4">
+        <v>679.43950000000007</v>
+      </c>
+      <c r="BK4">
+        <v>745.90750000000003</v>
+      </c>
+      <c r="BL4">
+        <v>735.85</v>
+      </c>
+      <c r="BM4">
+        <v>815.25</v>
+      </c>
+      <c r="BN4" s="41">
+        <f t="shared" ref="BN4:BN8" si="11">1-BL4/BJ4</f>
+        <v>-8.3025052267346799E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>256</v>
       </c>
@@ -15034,8 +15451,104 @@
         <f t="shared" si="0"/>
         <v>-0.16670224937456557</v>
       </c>
+      <c r="AK5">
+        <v>2079.7224999999999</v>
+      </c>
+      <c r="AL5">
+        <v>2185.6950000000002</v>
+      </c>
+      <c r="AM5">
+        <v>2113.0500000000002</v>
+      </c>
+      <c r="AN5">
+        <v>2249.6500000000005</v>
+      </c>
+      <c r="AO5" s="41">
+        <f t="shared" si="7"/>
+        <v>-1.6024974485778998E-2</v>
+      </c>
+      <c r="AP5">
+        <v>1711.3415</v>
+      </c>
+      <c r="AQ5">
+        <v>1912.9759999999999</v>
+      </c>
+      <c r="AR5">
+        <v>1618.75</v>
+      </c>
+      <c r="AS5">
+        <v>1842.4</v>
+      </c>
+      <c r="AT5" s="41">
+        <f t="shared" si="8"/>
+        <v>5.41046307823424E-2</v>
+      </c>
+      <c r="AU5">
+        <v>175.17</v>
+      </c>
+      <c r="AV5">
+        <v>195.11150000000001</v>
+      </c>
+      <c r="AW5">
+        <v>262.3</v>
+      </c>
+      <c r="AX5">
+        <v>309.65000000000003</v>
+      </c>
+      <c r="AY5" s="41">
+        <f t="shared" ref="AY5:AY9" si="12">1-AW5/AU5</f>
+        <v>-0.49740252326311607</v>
+      </c>
+      <c r="AZ5">
+        <v>7378.8629999999994</v>
+      </c>
+      <c r="BA5">
+        <v>7720.2284999999993</v>
+      </c>
+      <c r="BB5">
+        <v>10802.25</v>
+      </c>
+      <c r="BC5">
+        <v>11473.550000000001</v>
+      </c>
+      <c r="BD5" s="41">
+        <f t="shared" si="9"/>
+        <v>-0.46394505494952276</v>
+      </c>
+      <c r="BE5">
+        <v>1118.6774999999998</v>
+      </c>
+      <c r="BF5">
+        <v>1167.607</v>
+      </c>
+      <c r="BG5">
+        <v>1149.9000000000001</v>
+      </c>
+      <c r="BH5">
+        <v>1207.1000000000001</v>
+      </c>
+      <c r="BI5" s="41">
+        <f t="shared" si="10"/>
+        <v>-2.7910188593227581E-2</v>
+      </c>
+      <c r="BJ5">
+        <v>612.07749999999999</v>
+      </c>
+      <c r="BK5">
+        <v>676.92450000000008</v>
+      </c>
+      <c r="BL5">
+        <v>682.35</v>
+      </c>
+      <c r="BM5">
+        <v>794.65000000000009</v>
+      </c>
+      <c r="BN5" s="41">
+        <f t="shared" si="11"/>
+        <v>-0.11480980758155623</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>320</v>
       </c>
@@ -15151,8 +15664,104 @@
         <f t="shared" si="0"/>
         <v>-0.1784779109338468</v>
       </c>
+      <c r="AK6">
+        <v>2067.7199999999998</v>
+      </c>
+      <c r="AL6">
+        <v>2214.8685</v>
+      </c>
+      <c r="AM6">
+        <v>2076.6</v>
+      </c>
+      <c r="AN6">
+        <v>2275.0500000000002</v>
+      </c>
+      <c r="AO6" s="41">
+        <f t="shared" si="7"/>
+        <v>-4.2945853403748568E-3</v>
+      </c>
+      <c r="AP6">
+        <v>1636.1834999999996</v>
+      </c>
+      <c r="AQ6">
+        <v>1745.8910000000001</v>
+      </c>
+      <c r="AR6">
+        <v>1649.15</v>
+      </c>
+      <c r="AS6">
+        <v>1785.65</v>
+      </c>
+      <c r="AT6" s="41">
+        <f t="shared" si="8"/>
+        <v>-7.9248446155339991E-3</v>
+      </c>
+      <c r="AU6">
+        <v>176.49549999999999</v>
+      </c>
+      <c r="AV6">
+        <v>204.85200000000003</v>
+      </c>
+      <c r="AW6">
+        <v>265.75</v>
+      </c>
+      <c r="AX6">
+        <v>308.85000000000014</v>
+      </c>
+      <c r="AY6" s="41">
+        <f t="shared" si="12"/>
+        <v>-0.50570411143626903</v>
+      </c>
+      <c r="AZ6">
+        <v>5997.6269999999986</v>
+      </c>
+      <c r="BA6">
+        <v>6338.8050000000003</v>
+      </c>
+      <c r="BB6">
+        <v>8213.5</v>
+      </c>
+      <c r="BC6">
+        <v>8724.4</v>
+      </c>
+      <c r="BD6" s="41">
+        <f t="shared" si="9"/>
+        <v>-0.36945828741934128</v>
+      </c>
+      <c r="BE6">
+        <v>976.93249999999989</v>
+      </c>
+      <c r="BF6">
+        <v>1016.827</v>
+      </c>
+      <c r="BG6">
+        <v>1074</v>
+      </c>
+      <c r="BH6">
+        <v>1218.7500000000002</v>
+      </c>
+      <c r="BI6" s="41">
+        <f t="shared" si="10"/>
+        <v>-9.9359474682232607E-2</v>
+      </c>
+      <c r="BJ6">
+        <v>575.62950000000001</v>
+      </c>
+      <c r="BK6">
+        <v>623.96050000000014</v>
+      </c>
+      <c r="BL6">
+        <v>641.75</v>
+      </c>
+      <c r="BM6">
+        <v>705.7</v>
+      </c>
+      <c r="BN6" s="41">
+        <f t="shared" si="11"/>
+        <v>-0.11486642015393578</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>384</v>
       </c>
@@ -15268,8 +15877,104 @@
         <f t="shared" si="0"/>
         <v>-0.21739903141244921</v>
       </c>
+      <c r="AK7">
+        <v>2039.7484999999997</v>
+      </c>
+      <c r="AL7">
+        <v>2139.5095000000001</v>
+      </c>
+      <c r="AM7">
+        <v>2057</v>
+      </c>
+      <c r="AN7">
+        <v>2288.15</v>
+      </c>
+      <c r="AO7" s="41">
+        <f t="shared" si="7"/>
+        <v>-8.4576603439101561E-3</v>
+      </c>
+      <c r="AP7">
+        <v>1543.8185000000001</v>
+      </c>
+      <c r="AQ7">
+        <v>1679.702</v>
+      </c>
+      <c r="AR7">
+        <v>1577</v>
+      </c>
+      <c r="AS7">
+        <v>1692</v>
+      </c>
+      <c r="AT7" s="41">
+        <f t="shared" si="8"/>
+        <v>-2.1493135365329374E-2</v>
+      </c>
+      <c r="AU7">
+        <v>180.517</v>
+      </c>
+      <c r="AV7">
+        <v>221.34350000000003</v>
+      </c>
+      <c r="AW7">
+        <v>251.75</v>
+      </c>
+      <c r="AX7">
+        <v>304</v>
+      </c>
+      <c r="AY7" s="41">
+        <f t="shared" si="12"/>
+        <v>-0.39460549421938107</v>
+      </c>
+      <c r="AZ7">
+        <v>5008.7645000000002</v>
+      </c>
+      <c r="BA7">
+        <v>5275.5235000000002</v>
+      </c>
+      <c r="BB7">
+        <v>6890.9</v>
+      </c>
+      <c r="BC7">
+        <v>7406.35</v>
+      </c>
+      <c r="BD7" s="41">
+        <f t="shared" si="9"/>
+        <v>-0.37576841554439211</v>
+      </c>
+      <c r="BE7">
+        <v>890.97150000000022</v>
+      </c>
+      <c r="BF7">
+        <v>952.02100000000007</v>
+      </c>
+      <c r="BG7">
+        <v>958.35</v>
+      </c>
+      <c r="BH7">
+        <v>1013.0500000000002</v>
+      </c>
+      <c r="BI7" s="41">
+        <f t="shared" si="10"/>
+        <v>-7.5623631058905794E-2</v>
+      </c>
+      <c r="BJ7">
+        <v>554.44899999999996</v>
+      </c>
+      <c r="BK7">
+        <v>587.70650000000001</v>
+      </c>
+      <c r="BL7">
+        <v>627.25</v>
+      </c>
+      <c r="BM7">
+        <v>696.2</v>
+      </c>
+      <c r="BN7" s="41">
+        <f t="shared" si="11"/>
+        <v>-0.1313033299726396</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>448</v>
       </c>
@@ -15385,8 +16090,104 @@
         <f t="shared" si="0"/>
         <v>-0.2570320537249895</v>
       </c>
+      <c r="AK8">
+        <v>2071.4839999999995</v>
+      </c>
+      <c r="AL8">
+        <v>2200.9764999999998</v>
+      </c>
+      <c r="AM8">
+        <v>1917</v>
+      </c>
+      <c r="AN8">
+        <v>2006.45</v>
+      </c>
+      <c r="AO8" s="41">
+        <f t="shared" si="7"/>
+        <v>7.4576487194687235E-2</v>
+      </c>
+      <c r="AP8">
+        <v>1264.5909999999999</v>
+      </c>
+      <c r="AQ8">
+        <v>1353.326</v>
+      </c>
+      <c r="AR8">
+        <v>1583.45</v>
+      </c>
+      <c r="AS8">
+        <v>1797.05</v>
+      </c>
+      <c r="AT8" s="41">
+        <f t="shared" si="8"/>
+        <v>-0.25214397382236653</v>
+      </c>
+      <c r="AU8">
+        <v>182.02849999999995</v>
+      </c>
+      <c r="AV8">
+        <v>213.90750000000006</v>
+      </c>
+      <c r="AW8">
+        <v>249.1</v>
+      </c>
+      <c r="AX8">
+        <v>293.2</v>
+      </c>
+      <c r="AY8" s="41">
+        <f t="shared" si="12"/>
+        <v>-0.36846702576794321</v>
+      </c>
+      <c r="AZ8">
+        <v>4365.6729999999998</v>
+      </c>
+      <c r="BA8">
+        <v>4562.2420000000002</v>
+      </c>
+      <c r="BB8">
+        <v>6020.75</v>
+      </c>
+      <c r="BC8">
+        <v>6621</v>
+      </c>
+      <c r="BD8" s="41">
+        <f t="shared" si="9"/>
+        <v>-0.37911153675504328</v>
+      </c>
+      <c r="BE8">
+        <v>817.19049999999993</v>
+      </c>
+      <c r="BF8">
+        <v>867.0100000000001</v>
+      </c>
+      <c r="BG8">
+        <v>901.6</v>
+      </c>
+      <c r="BH8">
+        <v>992.40000000000009</v>
+      </c>
+      <c r="BI8" s="41">
+        <f t="shared" si="10"/>
+        <v>-0.10329231678537631</v>
+      </c>
+      <c r="BJ8">
+        <v>548.86550000000011</v>
+      </c>
+      <c r="BK8">
+        <v>585.60000000000025</v>
+      </c>
+      <c r="BL8">
+        <v>607.5</v>
+      </c>
+      <c r="BM8">
+        <v>687.55000000000007</v>
+      </c>
+      <c r="BN8" s="41">
+        <f t="shared" si="11"/>
+        <v>-0.10682853996106489</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>512</v>
       </c>
@@ -15502,8 +16303,96 @@
         <f>1-AH9/AF9</f>
         <v>-0.27706569106523049</v>
       </c>
+      <c r="AK9">
+        <v>2046.7869999999998</v>
+      </c>
+      <c r="AL9">
+        <v>2297.1005</v>
+      </c>
+      <c r="AM9" s="52">
+        <v>2072.85</v>
+      </c>
+      <c r="AN9" s="52">
+        <v>2241.0500000000002</v>
+      </c>
+      <c r="AO9" s="41">
+        <f t="shared" si="7"/>
+        <v>-1.2733616150581328E-2</v>
+      </c>
+      <c r="AP9">
+        <v>1257.5670000000002</v>
+      </c>
+      <c r="AQ9">
+        <v>1347.5364999999999</v>
+      </c>
+      <c r="AR9">
+        <v>1561.65</v>
+      </c>
+      <c r="AS9">
+        <v>1784.7500000000002</v>
+      </c>
+      <c r="AT9" s="41">
+        <f t="shared" si="8"/>
+        <v>-0.24180262363754768</v>
+      </c>
+      <c r="AU9">
+        <v>170.7895</v>
+      </c>
+      <c r="AV9">
+        <v>184.94299999999998</v>
+      </c>
+      <c r="AW9">
+        <v>252.25</v>
+      </c>
+      <c r="AX9">
+        <v>297.85000000000002</v>
+      </c>
+      <c r="AY9" s="41">
+        <f t="shared" si="12"/>
+        <v>-0.47696433328746779</v>
+      </c>
+      <c r="AZ9">
+        <v>3816.9615000000003</v>
+      </c>
+      <c r="BA9">
+        <v>3998.3964999999998</v>
+      </c>
+      <c r="BB9">
+        <v>5342.55</v>
+      </c>
+      <c r="BC9">
+        <v>5732.15</v>
+      </c>
+      <c r="BD9" s="41">
+        <f t="shared" si="9"/>
+        <v>-0.39968663556077244</v>
+      </c>
+      <c r="BE9">
+        <v>761.5089999999999</v>
+      </c>
+      <c r="BF9">
+        <v>786.12150000000008</v>
+      </c>
+      <c r="BG9">
+        <v>846.6</v>
+      </c>
+      <c r="BH9">
+        <v>881.50000000000011</v>
+      </c>
+      <c r="BI9" s="41">
+        <f t="shared" si="10"/>
+        <v>-0.11173997943556824</v>
+      </c>
+      <c r="BJ9">
+        <v>513.16099999999994</v>
+      </c>
+      <c r="BK9">
+        <v>568.25700000000006</v>
+      </c>
+      <c r="BL9" s="54"/>
+      <c r="BM9" s="54"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>576</v>
       </c>
@@ -15520,7 +16409,7 @@
         <v>1532.65</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>640</v>
       </c>
@@ -15537,7 +16426,7 @@
         <v>1423.65</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>704</v>
       </c>
@@ -15554,7 +16443,7 @@
         <v>1539.7500000000016</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>768</v>
       </c>
@@ -15571,7 +16460,7 @@
         <v>1407.0500000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>832</v>
       </c>
@@ -15588,7 +16477,7 @@
         <v>1396.1000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>896</v>
       </c>
@@ -15605,12 +16494,12 @@
         <v>1339.3500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>960</v>
       </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="33"/>
       <c r="Q16">
         <v>1</v>
@@ -15626,6 +16515,10 @@
       </c>
       <c r="AD16" s="42">
         <v>1609.3</v>
+      </c>
+      <c r="AQ16" s="27">
+        <f>(AN3-AL3)/AN3</f>
+        <v>0.10525041747559628</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
@@ -15647,7 +16540,7 @@
       <c r="AD17" s="42">
         <v>1340.7500000000002</v>
       </c>
-      <c r="AE17" s="73">
+      <c r="AE17" s="47">
         <f>1-AC17/AA17</f>
         <v>0.31162826847037239</v>
       </c>
@@ -15671,8 +16564,8 @@
       <c r="AD18" s="42">
         <v>1568.2999999999995</v>
       </c>
-      <c r="AE18" s="73">
-        <f t="shared" ref="AE18:AE24" si="7">1-AC18/AA18</f>
+      <c r="AE18" s="47">
+        <f t="shared" ref="AE18:AE23" si="13">1-AC18/AA18</f>
         <v>0.24684477040523256</v>
       </c>
     </row>
@@ -15695,8 +16588,8 @@
       <c r="AD19" s="42">
         <v>1409.8500000000001</v>
       </c>
-      <c r="AE19" s="73">
-        <f t="shared" si="7"/>
+      <c r="AE19" s="47">
+        <f t="shared" si="13"/>
         <v>0.24315813720468904</v>
       </c>
     </row>
@@ -15719,8 +16612,8 @@
       <c r="AD20" s="42">
         <v>1406</v>
       </c>
-      <c r="AE20" s="73">
-        <f t="shared" si="7"/>
+      <c r="AE20" s="47">
+        <f t="shared" si="13"/>
         <v>0.2107580828730059</v>
       </c>
     </row>
@@ -15743,8 +16636,8 @@
       <c r="AD21" s="42">
         <v>1361.3500000000001</v>
       </c>
-      <c r="AE21" s="73">
-        <f t="shared" si="7"/>
+      <c r="AE21" s="47">
+        <f t="shared" si="13"/>
         <v>0.18685773770110026</v>
       </c>
     </row>
@@ -15767,8 +16660,8 @@
       <c r="AD22" s="42">
         <v>1479.65</v>
       </c>
-      <c r="AE22" s="73">
-        <f t="shared" si="7"/>
+      <c r="AE22" s="47">
+        <f t="shared" si="13"/>
         <v>0.14910522848791985</v>
       </c>
     </row>
@@ -15791,8 +16684,8 @@
       <c r="AD23" s="42">
         <v>1381.3000000000002</v>
       </c>
-      <c r="AE23" s="73">
-        <f t="shared" si="7"/>
+      <c r="AE23" s="47">
+        <f t="shared" si="13"/>
         <v>0.12952252491603822</v>
       </c>
       <c r="AF23" t="s">
@@ -15818,11 +16711,11 @@
       <c r="AD24">
         <v>1574.75</v>
       </c>
-      <c r="AE24" s="73">
+      <c r="AE24" s="47">
         <f>1-AC24/AA24</f>
         <v>8.0012704851804672E-2</v>
       </c>
-      <c r="AF24" s="72">
+      <c r="AF24" s="46">
         <f>1-AD24/AB24</f>
         <v>-5.1915424597085646E-2</v>
       </c>
@@ -15850,7 +16743,7 @@
       <c r="AD25" s="42">
         <v>1429.6000000000001</v>
       </c>
-      <c r="AE25" s="73">
+      <c r="AE25" s="47">
         <f>1-AC25/AA25</f>
         <v>4.1469890556904421E-3</v>
       </c>
@@ -15878,7 +16771,7 @@
       <c r="AD26" s="44">
         <v>1251.3999999999999</v>
       </c>
-      <c r="AE26" s="73">
+      <c r="AE26" s="47">
         <f>1-AC26/AA26</f>
         <v>9.0658683266203743E-3</v>
       </c>
@@ -15985,14 +16878,19 @@
       <c r="B55" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
+  <mergeCells count="28">
+    <mergeCell ref="BJ1:BK1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="BG1:BH1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="A1:A2"/>
@@ -16002,6 +16900,13 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16024,20 +16929,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="69"/>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>